<commit_message>
issue 19 stained fixed tissue slide speimens
</commit_message>
<xml_diff>
--- a/src/external/ontoDog_input/ontoDog_input.xlsx
+++ b/src/external/ontoDog_input/ontoDog_input.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28028"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="3780" windowWidth="24240" windowHeight="13740"/>
+    <workbookView xWindow="1640" yWindow="540" windowWidth="30600" windowHeight="19320"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="262">
   <si>
     <t>Homo sapiens</t>
   </si>
@@ -789,6 +789,24 @@
   </si>
   <si>
     <t>is member of organization</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0302887</t>
+  </si>
+  <si>
+    <t>staining</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0002126</t>
+  </si>
+  <si>
+    <t>IHC-stained fixed tissue slide specimen</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0002125</t>
+  </si>
+  <si>
+    <t>H&amp;E-stained fixed tissue slide specimen</t>
   </si>
 </sst>
 </file>
@@ -837,8 +855,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -846,10 +866,12 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="6">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1149,22 +1171,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E125"/>
+  <dimension ref="A1:E128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="A129" sqref="A129"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C128" sqref="C128"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="57" customWidth="1"/>
-    <col min="2" max="2" width="49.140625" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="49.1640625" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>79</v>
       </c>
@@ -1181,7 +1203,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1192,7 +1214,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>95</v>
       </c>
@@ -1203,7 +1225,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1214,7 +1236,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1225,7 +1247,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1236,7 +1258,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1247,7 +1269,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1258,7 +1280,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1269,7 +1291,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1280,7 +1302,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1291,7 +1313,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>101</v>
       </c>
@@ -1305,7 +1327,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1316,7 +1338,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1327,7 +1349,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -1338,7 +1360,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>86</v>
       </c>
@@ -1349,7 +1371,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -1360,7 +1382,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -1371,7 +1393,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>88</v>
       </c>
@@ -1382,7 +1404,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -1393,7 +1415,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -1404,7 +1426,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -1415,7 +1437,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -1426,7 +1448,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -1437,7 +1459,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>44</v>
       </c>
@@ -1448,7 +1470,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -1459,7 +1481,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -1470,7 +1492,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>48</v>
       </c>
@@ -1481,7 +1503,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -1492,7 +1514,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
         <v>52</v>
       </c>
@@ -1503,7 +1525,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
         <v>103</v>
       </c>
@@ -1514,7 +1536,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
         <v>50</v>
       </c>
@@ -1525,7 +1547,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>58</v>
       </c>
@@ -1536,7 +1558,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>54</v>
       </c>
@@ -1547,7 +1569,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>56</v>
       </c>
@@ -1558,7 +1580,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>60</v>
       </c>
@@ -1569,7 +1591,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>62</v>
       </c>
@@ -1580,7 +1602,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>89</v>
       </c>
@@ -1591,7 +1613,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>93</v>
       </c>
@@ -1602,7 +1624,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>72</v>
       </c>
@@ -1613,7 +1635,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>70</v>
       </c>
@@ -1624,7 +1646,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
         <v>98</v>
       </c>
@@ -1635,7 +1657,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
         <v>68</v>
       </c>
@@ -1649,7 +1671,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
         <v>64</v>
       </c>
@@ -1660,7 +1682,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
         <v>74</v>
       </c>
@@ -1671,7 +1693,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
         <v>66</v>
       </c>
@@ -1682,7 +1704,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5">
       <c r="A47" t="s">
         <v>92</v>
       </c>
@@ -1693,7 +1715,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5">
       <c r="A48" t="s">
         <v>97</v>
       </c>
@@ -1704,7 +1726,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
         <v>76</v>
       </c>
@@ -1715,7 +1737,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
         <v>78</v>
       </c>
@@ -1726,7 +1748,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5">
       <c r="A51" t="s">
         <v>105</v>
       </c>
@@ -1737,7 +1759,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5">
       <c r="A52" t="s">
         <v>108</v>
       </c>
@@ -1748,7 +1770,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5">
       <c r="A53" t="s">
         <v>109</v>
       </c>
@@ -1762,7 +1784,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5">
       <c r="A54" t="s">
         <v>111</v>
       </c>
@@ -1773,7 +1795,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5">
       <c r="A55" t="s">
         <v>160</v>
       </c>
@@ -1784,7 +1806,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5">
       <c r="A56" t="s">
         <v>161</v>
       </c>
@@ -1795,7 +1817,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5">
       <c r="A57" t="s">
         <v>162</v>
       </c>
@@ -1806,7 +1828,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5">
       <c r="A58" t="s">
         <v>163</v>
       </c>
@@ -1817,7 +1839,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5">
       <c r="A59" t="s">
         <v>164</v>
       </c>
@@ -1828,7 +1850,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5">
       <c r="A60" t="s">
         <v>165</v>
       </c>
@@ -1839,7 +1861,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5">
       <c r="A61" t="s">
         <v>166</v>
       </c>
@@ -1850,7 +1872,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5">
       <c r="A62" t="s">
         <v>169</v>
       </c>
@@ -1861,7 +1883,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5">
       <c r="A63" t="s">
         <v>170</v>
       </c>
@@ -1872,7 +1894,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5">
       <c r="A64" t="s">
         <v>171</v>
       </c>
@@ -1883,7 +1905,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3">
       <c r="A65" t="s">
         <v>172</v>
       </c>
@@ -1894,7 +1916,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3">
       <c r="A66" t="s">
         <v>173</v>
       </c>
@@ -1905,7 +1927,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3">
       <c r="A67" t="s">
         <v>174</v>
       </c>
@@ -1916,7 +1938,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3">
       <c r="A68" t="s">
         <v>175</v>
       </c>
@@ -1927,7 +1949,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3">
       <c r="A69" t="s">
         <v>176</v>
       </c>
@@ -1938,7 +1960,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3">
       <c r="A70" t="s">
         <v>177</v>
       </c>
@@ -1949,7 +1971,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3">
       <c r="A71" t="s">
         <v>178</v>
       </c>
@@ -1960,7 +1982,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3">
       <c r="A72" t="s">
         <v>179</v>
       </c>
@@ -1971,7 +1993,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3">
       <c r="A73" t="s">
         <v>180</v>
       </c>
@@ -1982,7 +2004,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3">
       <c r="A74" t="s">
         <v>181</v>
       </c>
@@ -1993,7 +2015,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3">
       <c r="A75" t="s">
         <v>182</v>
       </c>
@@ -2004,7 +2026,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3">
       <c r="A76" t="s">
         <v>183</v>
       </c>
@@ -2015,7 +2037,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3">
       <c r="A77" t="s">
         <v>184</v>
       </c>
@@ -2026,7 +2048,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3">
       <c r="A78" t="s">
         <v>185</v>
       </c>
@@ -2037,7 +2059,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3">
       <c r="A79" t="s">
         <v>186</v>
       </c>
@@ -2048,7 +2070,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3">
       <c r="A80" t="s">
         <v>187</v>
       </c>
@@ -2059,7 +2081,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3">
       <c r="A81" t="s">
         <v>188</v>
       </c>
@@ -2070,7 +2092,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3">
       <c r="A82" t="s">
         <v>189</v>
       </c>
@@ -2081,7 +2103,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3">
       <c r="A83" t="s">
         <v>190</v>
       </c>
@@ -2092,7 +2114,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3">
       <c r="A84" t="s">
         <v>191</v>
       </c>
@@ -2103,7 +2125,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3">
       <c r="A85" t="s">
         <v>192</v>
       </c>
@@ -2114,7 +2136,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3">
       <c r="A86" t="s">
         <v>193</v>
       </c>
@@ -2125,7 +2147,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3">
       <c r="A87" t="s">
         <v>194</v>
       </c>
@@ -2136,7 +2158,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3">
       <c r="A88" t="s">
         <v>195</v>
       </c>
@@ -2147,7 +2169,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3">
       <c r="A89" t="s">
         <v>196</v>
       </c>
@@ -2158,7 +2180,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3">
       <c r="A90" t="s">
         <v>197</v>
       </c>
@@ -2169,7 +2191,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3">
       <c r="A91" t="s">
         <v>198</v>
       </c>
@@ -2180,7 +2202,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3">
       <c r="A92" t="s">
         <v>199</v>
       </c>
@@ -2191,7 +2213,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3">
       <c r="A93" t="s">
         <v>200</v>
       </c>
@@ -2202,7 +2224,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3">
       <c r="A94" t="s">
         <v>201</v>
       </c>
@@ -2213,7 +2235,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3">
       <c r="A95" t="s">
         <v>202</v>
       </c>
@@ -2224,7 +2246,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3">
       <c r="A96" t="s">
         <v>203</v>
       </c>
@@ -2235,7 +2257,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3">
       <c r="A97" t="s">
         <v>204</v>
       </c>
@@ -2246,7 +2268,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3">
       <c r="A98" t="s">
         <v>205</v>
       </c>
@@ -2257,7 +2279,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3">
       <c r="A99" t="s">
         <v>206</v>
       </c>
@@ -2268,7 +2290,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3">
       <c r="A100" t="s">
         <v>168</v>
       </c>
@@ -2279,7 +2301,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3">
       <c r="A101" t="s">
         <v>167</v>
       </c>
@@ -2290,7 +2312,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3">
       <c r="A102" t="s">
         <v>207</v>
       </c>
@@ -2301,7 +2323,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3">
       <c r="A103" t="s">
         <v>210</v>
       </c>
@@ -2312,7 +2334,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3">
       <c r="A104" t="s">
         <v>212</v>
       </c>
@@ -2323,7 +2345,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3">
       <c r="A105" t="s">
         <v>214</v>
       </c>
@@ -2334,7 +2356,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3">
       <c r="A106" t="s">
         <v>216</v>
       </c>
@@ -2345,7 +2367,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3">
       <c r="A107" t="s">
         <v>246</v>
       </c>
@@ -2356,7 +2378,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3">
       <c r="A108" t="s">
         <v>218</v>
       </c>
@@ -2367,7 +2389,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3">
       <c r="A109" t="s">
         <v>220</v>
       </c>
@@ -2378,7 +2400,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3">
       <c r="A110" t="s">
         <v>222</v>
       </c>
@@ -2389,7 +2411,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3">
       <c r="A111" t="s">
         <v>224</v>
       </c>
@@ -2400,7 +2422,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3">
       <c r="A112" t="s">
         <v>226</v>
       </c>
@@ -2411,7 +2433,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5">
       <c r="A113" t="s">
         <v>228</v>
       </c>
@@ -2422,7 +2444,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5">
       <c r="A114" t="s">
         <v>230</v>
       </c>
@@ -2433,7 +2455,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5">
       <c r="A115" t="s">
         <v>232</v>
       </c>
@@ -2444,7 +2466,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5">
       <c r="A116" t="s">
         <v>234</v>
       </c>
@@ -2455,7 +2477,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5">
       <c r="A117" t="s">
         <v>236</v>
       </c>
@@ -2466,7 +2488,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5">
       <c r="A118" t="s">
         <v>238</v>
       </c>
@@ -2477,7 +2499,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5">
       <c r="A119" t="s">
         <v>240</v>
       </c>
@@ -2488,7 +2510,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5">
       <c r="A120" t="s">
         <v>242</v>
       </c>
@@ -2499,7 +2521,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5">
       <c r="A121" t="s">
         <v>244</v>
       </c>
@@ -2510,7 +2532,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5">
       <c r="A122" t="s">
         <v>248</v>
       </c>
@@ -2521,7 +2543,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5">
       <c r="A123" t="s">
         <v>250</v>
       </c>
@@ -2532,7 +2554,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5">
       <c r="A124" t="s">
         <v>252</v>
       </c>
@@ -2543,7 +2565,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5">
       <c r="A125" t="s">
         <v>253</v>
       </c>
@@ -2551,6 +2573,42 @@
         <v>254</v>
       </c>
       <c r="C125" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5">
+      <c r="A126" t="s">
+        <v>256</v>
+      </c>
+      <c r="B126" t="s">
+        <v>257</v>
+      </c>
+      <c r="C126" t="s">
+        <v>85</v>
+      </c>
+      <c r="E126" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5">
+      <c r="A127" t="s">
+        <v>258</v>
+      </c>
+      <c r="B127" t="s">
+        <v>259</v>
+      </c>
+      <c r="C127" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5">
+      <c r="A128" t="s">
+        <v>260</v>
+      </c>
+      <c r="B128" t="s">
+        <v>261</v>
+      </c>
+      <c r="C128" t="s">
         <v>85</v>
       </c>
     </row>
@@ -2574,7 +2632,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -2591,7 +2649,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Adding terms from github issue 'NTR: a few imports #23'  Mark A. Miller, 2017-05-01 09:20 EDT
</commit_message>
<xml_diff>
--- a/src/external/ontoDog_input/ontoDog_input.xlsx
+++ b/src/external/ontoDog_input/ontoDog_input.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28028"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark Miller\ontology\src\external\ontoDog_input\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1640" yWindow="540" windowWidth="30600" windowHeight="19320"/>
+    <workbookView xWindow="1644" yWindow="540" windowWidth="30600" windowHeight="19320"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="268">
   <si>
     <t>Homo sapiens</t>
   </si>
@@ -807,12 +812,30 @@
   </si>
   <si>
     <t>H&amp;E-stained fixed tissue slide specimen</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/IAO_0000142</t>
+  </si>
+  <si>
+    <t>mentions</t>
+  </si>
+  <si>
+    <t>plan</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0000260</t>
+  </si>
+  <si>
+    <t>categorical value specification</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0001930</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -855,23 +878,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -879,6 +905,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1171,22 +1200,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E128"/>
+  <dimension ref="A1:E131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C128" sqref="C128"/>
+    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A132" sqref="A132"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="57" customWidth="1"/>
-    <col min="2" max="2" width="49.1640625" customWidth="1"/>
+    <col min="2" max="2" width="49.109375" customWidth="1"/>
     <col min="3" max="3" width="18.33203125" customWidth="1"/>
     <col min="4" max="4" width="22.6640625" customWidth="1"/>
-    <col min="5" max="5" width="19.5" customWidth="1"/>
+    <col min="5" max="5" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>79</v>
       </c>
@@ -1203,7 +1232,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1214,7 +1243,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>95</v>
       </c>
@@ -1225,7 +1254,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1236,7 +1265,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1247,7 +1276,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1258,7 +1287,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1269,7 +1298,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1280,7 +1309,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1291,7 +1320,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1302,7 +1331,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1313,7 +1342,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>101</v>
       </c>
@@ -1327,7 +1356,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1338,7 +1367,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1349,7 +1378,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -1360,7 +1389,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>86</v>
       </c>
@@ -1371,7 +1400,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -1382,7 +1411,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -1393,7 +1422,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>88</v>
       </c>
@@ -1404,7 +1433,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -1415,7 +1444,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -1426,7 +1455,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -1437,7 +1466,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -1448,7 +1477,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -1459,7 +1488,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>44</v>
       </c>
@@ -1470,7 +1499,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -1481,7 +1510,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -1492,7 +1521,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>48</v>
       </c>
@@ -1503,7 +1532,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -1514,7 +1543,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>52</v>
       </c>
@@ -1525,7 +1554,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>103</v>
       </c>
@@ -1536,7 +1565,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>50</v>
       </c>
@@ -1547,7 +1576,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>58</v>
       </c>
@@ -1558,7 +1587,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>54</v>
       </c>
@@ -1569,7 +1598,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>56</v>
       </c>
@@ -1580,7 +1609,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>60</v>
       </c>
@@ -1591,7 +1620,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>62</v>
       </c>
@@ -1602,7 +1631,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>89</v>
       </c>
@@ -1613,7 +1642,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>93</v>
       </c>
@@ -1624,7 +1653,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>72</v>
       </c>
@@ -1635,7 +1664,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>70</v>
       </c>
@@ -1646,7 +1675,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>98</v>
       </c>
@@ -1657,7 +1686,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>68</v>
       </c>
@@ -1671,7 +1700,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>64</v>
       </c>
@@ -1682,7 +1711,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>74</v>
       </c>
@@ -1693,7 +1722,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>66</v>
       </c>
@@ -1704,7 +1733,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>92</v>
       </c>
@@ -1715,7 +1744,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>97</v>
       </c>
@@ -1726,7 +1755,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>76</v>
       </c>
@@ -1737,7 +1766,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>78</v>
       </c>
@@ -1748,7 +1777,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>105</v>
       </c>
@@ -1759,7 +1788,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>108</v>
       </c>
@@ -1770,7 +1799,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>109</v>
       </c>
@@ -1784,7 +1813,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>111</v>
       </c>
@@ -1795,7 +1824,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>160</v>
       </c>
@@ -1806,7 +1835,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>161</v>
       </c>
@@ -1817,7 +1846,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>162</v>
       </c>
@@ -1828,7 +1857,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>163</v>
       </c>
@@ -1839,7 +1868,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>164</v>
       </c>
@@ -1850,7 +1879,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>165</v>
       </c>
@@ -1861,7 +1890,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>166</v>
       </c>
@@ -1872,7 +1901,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>169</v>
       </c>
@@ -1883,7 +1912,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>170</v>
       </c>
@@ -1894,7 +1923,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>171</v>
       </c>
@@ -1905,7 +1934,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>172</v>
       </c>
@@ -1916,7 +1945,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>173</v>
       </c>
@@ -1927,7 +1956,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>174</v>
       </c>
@@ -1938,7 +1967,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>175</v>
       </c>
@@ -1949,7 +1978,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>176</v>
       </c>
@@ -1960,7 +1989,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>177</v>
       </c>
@@ -1971,7 +2000,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>178</v>
       </c>
@@ -1982,7 +2011,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>179</v>
       </c>
@@ -1993,7 +2022,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>180</v>
       </c>
@@ -2004,7 +2033,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>181</v>
       </c>
@@ -2015,7 +2044,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>182</v>
       </c>
@@ -2026,7 +2055,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>183</v>
       </c>
@@ -2037,7 +2066,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>184</v>
       </c>
@@ -2048,7 +2077,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>185</v>
       </c>
@@ -2059,7 +2088,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>186</v>
       </c>
@@ -2070,7 +2099,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>187</v>
       </c>
@@ -2081,7 +2110,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>188</v>
       </c>
@@ -2092,7 +2121,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>189</v>
       </c>
@@ -2103,7 +2132,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>190</v>
       </c>
@@ -2114,7 +2143,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>191</v>
       </c>
@@ -2125,7 +2154,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>192</v>
       </c>
@@ -2136,7 +2165,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>193</v>
       </c>
@@ -2147,7 +2176,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>194</v>
       </c>
@@ -2158,7 +2187,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>195</v>
       </c>
@@ -2169,7 +2198,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>196</v>
       </c>
@@ -2180,7 +2209,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>197</v>
       </c>
@@ -2191,7 +2220,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>198</v>
       </c>
@@ -2202,7 +2231,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>199</v>
       </c>
@@ -2213,7 +2242,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="93" spans="1:3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>200</v>
       </c>
@@ -2224,7 +2253,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="94" spans="1:3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>201</v>
       </c>
@@ -2235,7 +2264,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="95" spans="1:3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>202</v>
       </c>
@@ -2246,7 +2275,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>203</v>
       </c>
@@ -2257,7 +2286,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>204</v>
       </c>
@@ -2268,7 +2297,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>205</v>
       </c>
@@ -2279,7 +2308,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="99" spans="1:3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>206</v>
       </c>
@@ -2290,7 +2319,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>168</v>
       </c>
@@ -2301,7 +2330,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="101" spans="1:3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>167</v>
       </c>
@@ -2312,7 +2341,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="102" spans="1:3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>207</v>
       </c>
@@ -2323,7 +2352,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="103" spans="1:3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>210</v>
       </c>
@@ -2334,7 +2363,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="104" spans="1:3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>212</v>
       </c>
@@ -2345,7 +2374,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="105" spans="1:3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>214</v>
       </c>
@@ -2356,7 +2385,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="106" spans="1:3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>216</v>
       </c>
@@ -2367,7 +2396,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="107" spans="1:3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>246</v>
       </c>
@@ -2378,7 +2407,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="108" spans="1:3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>218</v>
       </c>
@@ -2389,7 +2418,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="109" spans="1:3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>220</v>
       </c>
@@ -2400,7 +2429,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="110" spans="1:3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>222</v>
       </c>
@@ -2411,7 +2440,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="111" spans="1:3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>224</v>
       </c>
@@ -2422,7 +2451,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="112" spans="1:3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>226</v>
       </c>
@@ -2433,7 +2462,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>228</v>
       </c>
@@ -2444,7 +2473,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="114" spans="1:5">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>230</v>
       </c>
@@ -2455,7 +2484,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="115" spans="1:5">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>232</v>
       </c>
@@ -2466,7 +2495,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="116" spans="1:5">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>234</v>
       </c>
@@ -2477,7 +2506,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="117" spans="1:5">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>236</v>
       </c>
@@ -2488,7 +2517,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="118" spans="1:5">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>238</v>
       </c>
@@ -2499,7 +2528,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="119" spans="1:5">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>240</v>
       </c>
@@ -2510,7 +2539,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="120" spans="1:5">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>242</v>
       </c>
@@ -2521,7 +2550,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="121" spans="1:5">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>244</v>
       </c>
@@ -2532,7 +2561,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="122" spans="1:5">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>248</v>
       </c>
@@ -2543,7 +2572,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="123" spans="1:5">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>250</v>
       </c>
@@ -2554,7 +2583,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="124" spans="1:5">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>252</v>
       </c>
@@ -2565,7 +2594,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="125" spans="1:5">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>253</v>
       </c>
@@ -2576,7 +2605,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="126" spans="1:5">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>256</v>
       </c>
@@ -2590,7 +2619,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="127" spans="1:5">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>258</v>
       </c>
@@ -2601,7 +2630,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="128" spans="1:5">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>260</v>
       </c>
@@ -2609,6 +2638,39 @@
         <v>261</v>
       </c>
       <c r="C128" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A129" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B129" t="s">
+        <v>263</v>
+      </c>
+      <c r="C129" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A130" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B130" t="s">
+        <v>264</v>
+      </c>
+      <c r="C130" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A131" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C131" t="s">
         <v>85</v>
       </c>
     </row>
@@ -2616,8 +2678,14 @@
   <sortState ref="A2:E50">
     <sortCondition ref="B2:B50"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="A129" r:id="rId1"/>
+    <hyperlink ref="A130" r:id="rId2"/>
+    <hyperlink ref="A131" r:id="rId3"/>
+    <hyperlink ref="B131" r:id="rId4" display="http://purl.obolibrary.org/obo/OBI_0001930 categorical value specification"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2632,7 +2700,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -2649,7 +2717,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
BBRB OBI terms tracker issue 25
</commit_message>
<xml_diff>
--- a/src/external/ontoDog_input/ontoDog_input.xlsx
+++ b/src/external/ontoDog_input/ontoDog_input.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark Miller\ontology\src\external\ontoDog_input\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28028"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1644" yWindow="540" windowWidth="30600" windowHeight="19320"/>
+    <workbookView xWindow="3700" yWindow="0" windowWidth="29080" windowHeight="19840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="292">
   <si>
     <t>Homo sapiens</t>
   </si>
@@ -830,13 +825,85 @@
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/OBI_0001930</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0001064</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0400168</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0000852</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/IAO_0000129</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/IAO_0000329</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/IAO_0000305</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/IAO_0000414</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000005</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000027</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000196</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0000835</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/IAO_0000132</t>
+  </si>
+  <si>
+    <t>automatic tissue processor</t>
+  </si>
+  <si>
+    <t>microtome</t>
+  </si>
+  <si>
+    <t>record of missing knowledge</t>
+  </si>
+  <si>
+    <t>version number</t>
+  </si>
+  <si>
+    <t>running title</t>
+  </si>
+  <si>
+    <t>document title</t>
+  </si>
+  <si>
+    <t>mass measurement datum</t>
+  </si>
+  <si>
+    <t>temperature unit</t>
+  </si>
+  <si>
+    <t>degree celsius</t>
+  </si>
+  <si>
+    <t>pH</t>
+  </si>
+  <si>
+    <t>manufacturer</t>
+  </si>
+  <si>
+    <t>lot number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -859,6 +926,27 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -887,9 +975,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
@@ -1200,22 +1297,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E131"/>
+  <dimension ref="A1:E145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A132" sqref="A132"/>
+    <sheetView tabSelected="1" topLeftCell="A119" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A146" sqref="A146"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="57" customWidth="1"/>
-    <col min="2" max="2" width="49.109375" customWidth="1"/>
+    <col min="2" max="2" width="49.1640625" customWidth="1"/>
     <col min="3" max="3" width="18.33203125" customWidth="1"/>
     <col min="4" max="4" width="22.6640625" customWidth="1"/>
-    <col min="5" max="5" width="19.44140625" customWidth="1"/>
+    <col min="5" max="5" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>79</v>
       </c>
@@ -1232,7 +1329,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1243,7 +1340,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>95</v>
       </c>
@@ -1254,7 +1351,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1265,7 +1362,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1276,7 +1373,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1287,7 +1384,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1298,7 +1395,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1309,7 +1406,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1320,7 +1417,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1331,7 +1428,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1342,7 +1439,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>101</v>
       </c>
@@ -1356,7 +1453,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1367,7 +1464,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1378,7 +1475,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -1389,7 +1486,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>86</v>
       </c>
@@ -1399,8 +1496,11 @@
       <c r="C16" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -1411,7 +1511,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -1422,7 +1522,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>88</v>
       </c>
@@ -1433,7 +1533,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -1444,7 +1544,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -1455,7 +1555,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -1466,7 +1566,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -1477,7 +1577,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -1488,7 +1588,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>44</v>
       </c>
@@ -1499,7 +1599,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -1510,7 +1610,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -1521,7 +1621,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>48</v>
       </c>
@@ -1532,7 +1632,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -1543,7 +1643,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
         <v>52</v>
       </c>
@@ -1554,7 +1654,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
         <v>103</v>
       </c>
@@ -1565,7 +1665,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
         <v>50</v>
       </c>
@@ -1576,7 +1676,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>58</v>
       </c>
@@ -1587,7 +1687,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>54</v>
       </c>
@@ -1598,7 +1698,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>56</v>
       </c>
@@ -1609,7 +1709,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>60</v>
       </c>
@@ -1620,7 +1720,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>62</v>
       </c>
@@ -1631,7 +1731,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>89</v>
       </c>
@@ -1642,7 +1742,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>93</v>
       </c>
@@ -1653,7 +1753,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>72</v>
       </c>
@@ -1664,7 +1764,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>70</v>
       </c>
@@ -1675,7 +1775,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
         <v>98</v>
       </c>
@@ -1686,7 +1786,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
         <v>68</v>
       </c>
@@ -1700,7 +1800,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
         <v>64</v>
       </c>
@@ -1711,7 +1811,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
         <v>74</v>
       </c>
@@ -1722,7 +1822,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
         <v>66</v>
       </c>
@@ -1733,7 +1833,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5">
       <c r="A47" t="s">
         <v>92</v>
       </c>
@@ -1744,7 +1844,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5">
       <c r="A48" t="s">
         <v>97</v>
       </c>
@@ -1755,7 +1855,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
         <v>76</v>
       </c>
@@ -1766,7 +1866,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
         <v>78</v>
       </c>
@@ -1777,7 +1877,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5">
       <c r="A51" t="s">
         <v>105</v>
       </c>
@@ -1788,7 +1888,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5">
       <c r="A52" t="s">
         <v>108</v>
       </c>
@@ -1799,7 +1899,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5">
       <c r="A53" t="s">
         <v>109</v>
       </c>
@@ -1813,7 +1913,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5">
       <c r="A54" t="s">
         <v>111</v>
       </c>
@@ -1824,7 +1924,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5">
       <c r="A55" t="s">
         <v>160</v>
       </c>
@@ -1835,7 +1935,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5">
       <c r="A56" t="s">
         <v>161</v>
       </c>
@@ -1846,7 +1946,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5">
       <c r="A57" t="s">
         <v>162</v>
       </c>
@@ -1857,7 +1957,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5">
       <c r="A58" t="s">
         <v>163</v>
       </c>
@@ -1868,7 +1968,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5">
       <c r="A59" t="s">
         <v>164</v>
       </c>
@@ -1879,7 +1979,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5">
       <c r="A60" t="s">
         <v>165</v>
       </c>
@@ -1890,7 +1990,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5">
       <c r="A61" t="s">
         <v>166</v>
       </c>
@@ -1901,7 +2001,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5">
       <c r="A62" t="s">
         <v>169</v>
       </c>
@@ -1912,7 +2012,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5">
       <c r="A63" t="s">
         <v>170</v>
       </c>
@@ -1923,7 +2023,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5">
       <c r="A64" t="s">
         <v>171</v>
       </c>
@@ -1934,7 +2034,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3">
       <c r="A65" t="s">
         <v>172</v>
       </c>
@@ -1945,7 +2045,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3">
       <c r="A66" t="s">
         <v>173</v>
       </c>
@@ -1956,7 +2056,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3">
       <c r="A67" t="s">
         <v>174</v>
       </c>
@@ -1967,7 +2067,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3">
       <c r="A68" t="s">
         <v>175</v>
       </c>
@@ -1978,7 +2078,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3">
       <c r="A69" t="s">
         <v>176</v>
       </c>
@@ -1989,7 +2089,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3">
       <c r="A70" t="s">
         <v>177</v>
       </c>
@@ -2000,7 +2100,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3">
       <c r="A71" t="s">
         <v>178</v>
       </c>
@@ -2011,7 +2111,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3">
       <c r="A72" t="s">
         <v>179</v>
       </c>
@@ -2022,7 +2122,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3">
       <c r="A73" t="s">
         <v>180</v>
       </c>
@@ -2033,7 +2133,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3">
       <c r="A74" t="s">
         <v>181</v>
       </c>
@@ -2044,7 +2144,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3">
       <c r="A75" t="s">
         <v>182</v>
       </c>
@@ -2055,7 +2155,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3">
       <c r="A76" t="s">
         <v>183</v>
       </c>
@@ -2066,7 +2166,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3">
       <c r="A77" t="s">
         <v>184</v>
       </c>
@@ -2077,7 +2177,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3">
       <c r="A78" t="s">
         <v>185</v>
       </c>
@@ -2088,7 +2188,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3">
       <c r="A79" t="s">
         <v>186</v>
       </c>
@@ -2099,7 +2199,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3">
       <c r="A80" t="s">
         <v>187</v>
       </c>
@@ -2110,7 +2210,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3">
       <c r="A81" t="s">
         <v>188</v>
       </c>
@@ -2121,7 +2221,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3">
       <c r="A82" t="s">
         <v>189</v>
       </c>
@@ -2132,7 +2232,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3">
       <c r="A83" t="s">
         <v>190</v>
       </c>
@@ -2143,7 +2243,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3">
       <c r="A84" t="s">
         <v>191</v>
       </c>
@@ -2154,7 +2254,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3">
       <c r="A85" t="s">
         <v>192</v>
       </c>
@@ -2165,7 +2265,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3">
       <c r="A86" t="s">
         <v>193</v>
       </c>
@@ -2176,7 +2276,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3">
       <c r="A87" t="s">
         <v>194</v>
       </c>
@@ -2187,7 +2287,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3">
       <c r="A88" t="s">
         <v>195</v>
       </c>
@@ -2198,7 +2298,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3">
       <c r="A89" t="s">
         <v>196</v>
       </c>
@@ -2209,7 +2309,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3">
       <c r="A90" t="s">
         <v>197</v>
       </c>
@@ -2220,7 +2320,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3">
       <c r="A91" t="s">
         <v>198</v>
       </c>
@@ -2231,7 +2331,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3">
       <c r="A92" t="s">
         <v>199</v>
       </c>
@@ -2242,7 +2342,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3">
       <c r="A93" t="s">
         <v>200</v>
       </c>
@@ -2253,7 +2353,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3">
       <c r="A94" t="s">
         <v>201</v>
       </c>
@@ -2264,7 +2364,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3">
       <c r="A95" t="s">
         <v>202</v>
       </c>
@@ -2275,7 +2375,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3">
       <c r="A96" t="s">
         <v>203</v>
       </c>
@@ -2286,7 +2386,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3">
       <c r="A97" t="s">
         <v>204</v>
       </c>
@@ -2297,7 +2397,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3">
       <c r="A98" t="s">
         <v>205</v>
       </c>
@@ -2308,7 +2408,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3">
       <c r="A99" t="s">
         <v>206</v>
       </c>
@@ -2319,7 +2419,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3">
       <c r="A100" t="s">
         <v>168</v>
       </c>
@@ -2330,7 +2430,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3">
       <c r="A101" t="s">
         <v>167</v>
       </c>
@@ -2341,7 +2441,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3">
       <c r="A102" t="s">
         <v>207</v>
       </c>
@@ -2352,7 +2452,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3">
       <c r="A103" t="s">
         <v>210</v>
       </c>
@@ -2363,7 +2463,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3">
       <c r="A104" t="s">
         <v>212</v>
       </c>
@@ -2374,7 +2474,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3">
       <c r="A105" t="s">
         <v>214</v>
       </c>
@@ -2385,7 +2485,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3">
       <c r="A106" t="s">
         <v>216</v>
       </c>
@@ -2396,7 +2496,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3">
       <c r="A107" t="s">
         <v>246</v>
       </c>
@@ -2407,7 +2507,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3">
       <c r="A108" t="s">
         <v>218</v>
       </c>
@@ -2418,7 +2518,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3">
       <c r="A109" t="s">
         <v>220</v>
       </c>
@@ -2429,7 +2529,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3">
       <c r="A110" t="s">
         <v>222</v>
       </c>
@@ -2440,7 +2540,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3">
       <c r="A111" t="s">
         <v>224</v>
       </c>
@@ -2451,7 +2551,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3">
       <c r="A112" t="s">
         <v>226</v>
       </c>
@@ -2462,7 +2562,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5">
       <c r="A113" t="s">
         <v>228</v>
       </c>
@@ -2473,7 +2573,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5">
       <c r="A114" t="s">
         <v>230</v>
       </c>
@@ -2484,7 +2584,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5">
       <c r="A115" t="s">
         <v>232</v>
       </c>
@@ -2495,7 +2595,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5">
       <c r="A116" t="s">
         <v>234</v>
       </c>
@@ -2506,7 +2606,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5">
       <c r="A117" t="s">
         <v>236</v>
       </c>
@@ -2517,7 +2617,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5">
       <c r="A118" t="s">
         <v>238</v>
       </c>
@@ -2528,7 +2628,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5">
       <c r="A119" t="s">
         <v>240</v>
       </c>
@@ -2539,7 +2639,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5">
       <c r="A120" t="s">
         <v>242</v>
       </c>
@@ -2550,7 +2650,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5">
       <c r="A121" t="s">
         <v>244</v>
       </c>
@@ -2561,7 +2661,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5">
       <c r="A122" t="s">
         <v>248</v>
       </c>
@@ -2572,7 +2672,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5">
       <c r="A123" t="s">
         <v>250</v>
       </c>
@@ -2583,7 +2683,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5">
       <c r="A124" t="s">
         <v>252</v>
       </c>
@@ -2594,7 +2694,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5">
       <c r="A125" t="s">
         <v>253</v>
       </c>
@@ -2605,7 +2705,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5">
       <c r="A126" t="s">
         <v>256</v>
       </c>
@@ -2619,7 +2719,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5">
       <c r="A127" t="s">
         <v>258</v>
       </c>
@@ -2630,7 +2730,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5">
       <c r="A128" t="s">
         <v>260</v>
       </c>
@@ -2641,7 +2741,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:3">
       <c r="A129" s="1" t="s">
         <v>262</v>
       </c>
@@ -2652,7 +2752,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:3">
       <c r="A130" s="1" t="s">
         <v>265</v>
       </c>
@@ -2663,7 +2763,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:3">
       <c r="A131" s="1" t="s">
         <v>267</v>
       </c>
@@ -2673,6 +2773,144 @@
       <c r="C131" t="s">
         <v>85</v>
       </c>
+    </row>
+    <row r="132" spans="1:3">
+      <c r="A132" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="B132" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="C132" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B133" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="C133" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B134" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="C134" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="A135" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B135" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="C135" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B136" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C136" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B137" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="C137" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="B138" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C138" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="B139" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="C139" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="B140" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="C140" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="A141" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="B141" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="C141" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="B142" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="C142" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="A143" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="B143" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="C143" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="B144" s="6"/>
+    </row>
+    <row r="145" spans="2:2">
+      <c r="B145" s="6"/>
     </row>
   </sheetData>
   <sortState ref="A2:E50">
@@ -2683,9 +2921,21 @@
     <hyperlink ref="A130" r:id="rId2"/>
     <hyperlink ref="A131" r:id="rId3"/>
     <hyperlink ref="B131" r:id="rId4" display="http://purl.obolibrary.org/obo/OBI_0001930 categorical value specification"/>
+    <hyperlink ref="A132" r:id="rId5"/>
+    <hyperlink ref="A133" r:id="rId6"/>
+    <hyperlink ref="A134" r:id="rId7"/>
+    <hyperlink ref="A135" r:id="rId8"/>
+    <hyperlink ref="A136" r:id="rId9"/>
+    <hyperlink ref="A137" r:id="rId10"/>
+    <hyperlink ref="A138" r:id="rId11"/>
+    <hyperlink ref="A139" r:id="rId12"/>
+    <hyperlink ref="A140" r:id="rId13"/>
+    <hyperlink ref="A141" r:id="rId14"/>
+    <hyperlink ref="A142" r:id="rId15"/>
+    <hyperlink ref="A143" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2700,7 +2950,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -2717,7 +2967,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
added BBRB requested terms from OBI tracker items #823,#824,#825,#834,#835
</commit_message>
<xml_diff>
--- a/src/external/ontoDog_input/ontoDog_input.xlsx
+++ b/src/external/ontoDog_input/ontoDog_input.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26606"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stoeckrtTM/Git/biobanking-ontology/ontology/src/external/ontoDog_input/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2220" yWindow="1640" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="-26000" yWindow="6980" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="360">
   <si>
     <t>Homo sapiens</t>
   </si>
@@ -927,13 +932,187 @@
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/OBI_0000651</t>
+  </si>
+  <si>
+    <t>cell pellet</t>
+  </si>
+  <si>
+    <t>material transport service</t>
+  </si>
+  <si>
+    <t>service</t>
+  </si>
+  <si>
+    <t>service provider role</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_1000024</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0001580</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0001173</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0000947</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000195</t>
+  </si>
+  <si>
+    <t>degree Fahrenheit</t>
+  </si>
+  <si>
+    <t>RNA Integrity Number calculation</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0002136</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0002137</t>
+  </si>
+  <si>
+    <t>RNA Integrity Number value specification</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0002145</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0002155</t>
+  </si>
+  <si>
+    <t>venereal disease research laboratory test</t>
+  </si>
+  <si>
+    <t>antigen specific antibodies assay</t>
+  </si>
+  <si>
+    <t>rapid plasma reagin test</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0002156</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0002157</t>
+  </si>
+  <si>
+    <t>HBV surface antigen test</t>
+  </si>
+  <si>
+    <t>HIV-1 nucleic acid testing</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0002158</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0002159</t>
+  </si>
+  <si>
+    <t>HCV nucleic acid testing</t>
+  </si>
+  <si>
+    <t>temperature value specification</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0002138</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0002139</t>
+  </si>
+  <si>
+    <t>volume value specification</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0002140</t>
+  </si>
+  <si>
+    <t>temperature measurement assay</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0002141</t>
+  </si>
+  <si>
+    <t>volume measurement assay</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0002543</t>
+  </si>
+  <si>
+    <t>atrial appendage specimen</t>
+  </si>
+  <si>
+    <t>esophagogastric junction specimen</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0002544</t>
+  </si>
+  <si>
+    <t>ileum specimen</t>
+  </si>
+  <si>
+    <t>liver specimen</t>
+  </si>
+  <si>
+    <t>minor salivary gland specimen</t>
+  </si>
+  <si>
+    <t>omentum specimen</t>
+  </si>
+  <si>
+    <t>ovary specimen</t>
+  </si>
+  <si>
+    <t>sigmoid colon specimen</t>
+  </si>
+  <si>
+    <t>suprapubic skin specimen</t>
+  </si>
+  <si>
+    <t>testis specimen</t>
+  </si>
+  <si>
+    <t>uterus specimen</t>
+  </si>
+  <si>
+    <t>vagina specimen</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0002545</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0002546</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0002547</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0002548</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0002549</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0002550</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0002551</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0002552</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0002553</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0002554</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -978,6 +1157,11 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1005,7 +1189,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1017,6 +1201,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
@@ -1327,13 +1515,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E148"/>
+  <dimension ref="A1:E177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A150" sqref="A150"/>
+    <sheetView tabSelected="1" topLeftCell="A155" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A178" sqref="A178"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="57" customWidth="1"/>
     <col min="2" max="2" width="49.1640625" customWidth="1"/>
@@ -1342,7 +1530,7 @@
     <col min="5" max="5" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>79</v>
       </c>
@@ -1359,7 +1547,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1370,7 +1558,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>95</v>
       </c>
@@ -1381,7 +1569,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1392,7 +1580,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1403,7 +1591,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1414,7 +1602,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1425,7 +1613,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1436,7 +1624,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1447,7 +1635,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1458,7 +1646,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1469,7 +1657,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>101</v>
       </c>
@@ -1483,7 +1671,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1494,7 +1682,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1505,7 +1693,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -1516,7 +1704,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>86</v>
       </c>
@@ -1530,7 +1718,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -1541,7 +1729,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -1552,7 +1740,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>88</v>
       </c>
@@ -1563,7 +1751,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -1574,7 +1762,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -1585,7 +1773,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -1596,7 +1784,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -1607,7 +1795,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -1618,7 +1806,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>44</v>
       </c>
@@ -1629,7 +1817,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -1640,7 +1828,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -1651,7 +1839,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>48</v>
       </c>
@@ -1662,7 +1850,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -1673,7 +1861,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>52</v>
       </c>
@@ -1684,7 +1872,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>103</v>
       </c>
@@ -1695,7 +1883,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>50</v>
       </c>
@@ -1706,7 +1894,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>58</v>
       </c>
@@ -1717,7 +1905,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>54</v>
       </c>
@@ -1728,7 +1916,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>56</v>
       </c>
@@ -1739,7 +1927,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>60</v>
       </c>
@@ -1750,7 +1938,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>62</v>
       </c>
@@ -1761,7 +1949,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>89</v>
       </c>
@@ -1772,7 +1960,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>93</v>
       </c>
@@ -1783,7 +1971,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>72</v>
       </c>
@@ -1794,7 +1982,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>70</v>
       </c>
@@ -1805,7 +1993,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>98</v>
       </c>
@@ -1816,7 +2004,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>68</v>
       </c>
@@ -1830,7 +2018,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>64</v>
       </c>
@@ -1841,7 +2029,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>74</v>
       </c>
@@ -1852,7 +2040,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>66</v>
       </c>
@@ -1863,7 +2051,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>92</v>
       </c>
@@ -1874,7 +2062,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>97</v>
       </c>
@@ -1885,7 +2073,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>76</v>
       </c>
@@ -1896,7 +2084,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>78</v>
       </c>
@@ -1907,7 +2095,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>105</v>
       </c>
@@ -1918,7 +2106,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>108</v>
       </c>
@@ -1929,7 +2117,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>109</v>
       </c>
@@ -1943,7 +2131,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>111</v>
       </c>
@@ -1954,7 +2142,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>160</v>
       </c>
@@ -1965,7 +2153,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>161</v>
       </c>
@@ -1976,7 +2164,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>162</v>
       </c>
@@ -1987,7 +2175,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>163</v>
       </c>
@@ -1998,7 +2186,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>164</v>
       </c>
@@ -2009,7 +2197,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>165</v>
       </c>
@@ -2020,7 +2208,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>166</v>
       </c>
@@ -2031,7 +2219,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>169</v>
       </c>
@@ -2042,7 +2230,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>170</v>
       </c>
@@ -2053,7 +2241,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>171</v>
       </c>
@@ -2064,7 +2252,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>172</v>
       </c>
@@ -2075,7 +2263,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>173</v>
       </c>
@@ -2086,7 +2274,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>174</v>
       </c>
@@ -2097,7 +2285,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>175</v>
       </c>
@@ -2108,7 +2296,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>176</v>
       </c>
@@ -2119,7 +2307,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>177</v>
       </c>
@@ -2130,7 +2318,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>178</v>
       </c>
@@ -2141,7 +2329,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>179</v>
       </c>
@@ -2152,7 +2340,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>180</v>
       </c>
@@ -2163,7 +2351,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>181</v>
       </c>
@@ -2174,7 +2362,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>182</v>
       </c>
@@ -2185,7 +2373,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>183</v>
       </c>
@@ -2196,7 +2384,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>184</v>
       </c>
@@ -2207,7 +2395,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>185</v>
       </c>
@@ -2218,7 +2406,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>186</v>
       </c>
@@ -2229,7 +2417,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>187</v>
       </c>
@@ -2240,7 +2428,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>188</v>
       </c>
@@ -2251,7 +2439,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>189</v>
       </c>
@@ -2262,7 +2450,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>190</v>
       </c>
@@ -2273,7 +2461,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>191</v>
       </c>
@@ -2284,7 +2472,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>192</v>
       </c>
@@ -2295,7 +2483,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>193</v>
       </c>
@@ -2306,7 +2494,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>194</v>
       </c>
@@ -2317,7 +2505,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>195</v>
       </c>
@@ -2328,7 +2516,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>196</v>
       </c>
@@ -2339,7 +2527,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>197</v>
       </c>
@@ -2350,7 +2538,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>198</v>
       </c>
@@ -2361,7 +2549,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>199</v>
       </c>
@@ -2372,7 +2560,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="93" spans="1:3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>200</v>
       </c>
@@ -2383,7 +2571,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="94" spans="1:3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>201</v>
       </c>
@@ -2394,7 +2582,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="95" spans="1:3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>202</v>
       </c>
@@ -2405,7 +2593,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>203</v>
       </c>
@@ -2416,7 +2604,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>204</v>
       </c>
@@ -2427,7 +2615,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>205</v>
       </c>
@@ -2438,7 +2626,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="99" spans="1:3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>206</v>
       </c>
@@ -2449,7 +2637,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>168</v>
       </c>
@@ -2460,7 +2648,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="101" spans="1:3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>167</v>
       </c>
@@ -2471,7 +2659,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="102" spans="1:3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>207</v>
       </c>
@@ -2482,7 +2670,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="103" spans="1:3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>210</v>
       </c>
@@ -2493,7 +2681,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="104" spans="1:3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>212</v>
       </c>
@@ -2504,7 +2692,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="105" spans="1:3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>214</v>
       </c>
@@ -2515,7 +2703,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="106" spans="1:3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>216</v>
       </c>
@@ -2526,7 +2714,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="107" spans="1:3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>246</v>
       </c>
@@ -2537,7 +2725,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="108" spans="1:3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>218</v>
       </c>
@@ -2548,7 +2736,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="109" spans="1:3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>220</v>
       </c>
@@ -2559,7 +2747,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="110" spans="1:3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>222</v>
       </c>
@@ -2570,7 +2758,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="111" spans="1:3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>224</v>
       </c>
@@ -2581,7 +2769,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="112" spans="1:3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>226</v>
       </c>
@@ -2592,7 +2780,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>228</v>
       </c>
@@ -2603,7 +2791,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="114" spans="1:5">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>230</v>
       </c>
@@ -2614,7 +2802,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="115" spans="1:5">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>232</v>
       </c>
@@ -2625,7 +2813,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="116" spans="1:5">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>234</v>
       </c>
@@ -2636,7 +2824,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="117" spans="1:5">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>236</v>
       </c>
@@ -2647,7 +2835,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="118" spans="1:5">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>238</v>
       </c>
@@ -2658,7 +2846,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="119" spans="1:5">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>240</v>
       </c>
@@ -2669,7 +2857,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="120" spans="1:5">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>242</v>
       </c>
@@ -2680,7 +2868,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="121" spans="1:5">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>244</v>
       </c>
@@ -2691,7 +2879,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="122" spans="1:5">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>248</v>
       </c>
@@ -2702,7 +2890,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="123" spans="1:5">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>250</v>
       </c>
@@ -2713,7 +2901,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="124" spans="1:5">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>252</v>
       </c>
@@ -2724,7 +2912,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="125" spans="1:5">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>253</v>
       </c>
@@ -2735,7 +2923,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="126" spans="1:5">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>256</v>
       </c>
@@ -2749,7 +2937,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="127" spans="1:5">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>258</v>
       </c>
@@ -2760,7 +2948,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="128" spans="1:5">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>260</v>
       </c>
@@ -2771,7 +2959,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="129" spans="1:3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>262</v>
       </c>
@@ -2782,7 +2970,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="130" spans="1:3">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>265</v>
       </c>
@@ -2793,7 +2981,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="131" spans="1:3">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>267</v>
       </c>
@@ -2804,7 +2992,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="132" spans="1:3">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
         <v>268</v>
       </c>
@@ -2815,7 +3003,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="133" spans="1:3">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
         <v>269</v>
       </c>
@@ -2826,7 +3014,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="134" spans="1:3">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
         <v>270</v>
       </c>
@@ -2837,7 +3025,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="135" spans="1:3">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
         <v>271</v>
       </c>
@@ -2848,7 +3036,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="136" spans="1:3">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
         <v>272</v>
       </c>
@@ -2859,7 +3047,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="137" spans="1:3">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
         <v>273</v>
       </c>
@@ -2870,7 +3058,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="138" spans="1:3">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
         <v>274</v>
       </c>
@@ -2881,7 +3069,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="139" spans="1:3">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" s="3" t="s">
         <v>275</v>
       </c>
@@ -2892,7 +3080,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="140" spans="1:3">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" s="3" t="s">
         <v>276</v>
       </c>
@@ -2903,7 +3091,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="141" spans="1:3">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" s="3" t="s">
         <v>277</v>
       </c>
@@ -2914,7 +3102,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="142" spans="1:3">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" s="3" t="s">
         <v>278</v>
       </c>
@@ -2925,7 +3113,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="143" spans="1:3">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" s="3" t="s">
         <v>279</v>
       </c>
@@ -2936,7 +3124,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="144" spans="1:3">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>292</v>
       </c>
@@ -2947,7 +3135,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="145" spans="1:3">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>294</v>
       </c>
@@ -2958,7 +3146,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="146" spans="1:3">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>296</v>
       </c>
@@ -2969,7 +3157,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="147" spans="1:3">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>300</v>
       </c>
@@ -2980,7 +3168,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="148" spans="1:3">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>301</v>
       </c>
@@ -2988,6 +3176,328 @@
         <v>299</v>
       </c>
       <c r="C148" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A149" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B149" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="C149" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A150" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B150" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="C150" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A151" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B151" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="C151" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A152" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="B152" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="C152" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>310</v>
+      </c>
+      <c r="B153" t="s">
+        <v>311</v>
+      </c>
+      <c r="C153" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>313</v>
+      </c>
+      <c r="B154" t="s">
+        <v>312</v>
+      </c>
+      <c r="C154" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>314</v>
+      </c>
+      <c r="B155" t="s">
+        <v>315</v>
+      </c>
+      <c r="C155" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>316</v>
+      </c>
+      <c r="B156" t="s">
+        <v>319</v>
+      </c>
+      <c r="C156" t="s">
+        <v>85</v>
+      </c>
+      <c r="E156" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>317</v>
+      </c>
+      <c r="B157" t="s">
+        <v>318</v>
+      </c>
+      <c r="C157" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>321</v>
+      </c>
+      <c r="B158" t="s">
+        <v>320</v>
+      </c>
+      <c r="C158" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>322</v>
+      </c>
+      <c r="B159" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="C159" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>325</v>
+      </c>
+      <c r="B160" t="s">
+        <v>324</v>
+      </c>
+      <c r="C160" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>326</v>
+      </c>
+      <c r="B161" t="s">
+        <v>327</v>
+      </c>
+      <c r="C161" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>329</v>
+      </c>
+      <c r="B162" t="s">
+        <v>328</v>
+      </c>
+      <c r="C162" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>330</v>
+      </c>
+      <c r="B163" t="s">
+        <v>331</v>
+      </c>
+      <c r="C163" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>332</v>
+      </c>
+      <c r="B164" t="s">
+        <v>333</v>
+      </c>
+      <c r="C164" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A165" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B165" t="s">
+        <v>335</v>
+      </c>
+      <c r="C165" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>336</v>
+      </c>
+      <c r="B166" t="s">
+        <v>337</v>
+      </c>
+      <c r="C166" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>339</v>
+      </c>
+      <c r="B167" t="s">
+        <v>338</v>
+      </c>
+      <c r="C167" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A168" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B168" t="s">
+        <v>340</v>
+      </c>
+      <c r="C168" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A169" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B169" t="s">
+        <v>341</v>
+      </c>
+      <c r="C169" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A170" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="B170" t="s">
+        <v>342</v>
+      </c>
+      <c r="C170" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A171" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B171" t="s">
+        <v>343</v>
+      </c>
+      <c r="C171" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A172" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="B172" t="s">
+        <v>344</v>
+      </c>
+      <c r="C172" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A173" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B173" t="s">
+        <v>345</v>
+      </c>
+      <c r="C173" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A174" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B174" t="s">
+        <v>346</v>
+      </c>
+      <c r="C174" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A175" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="B175" t="s">
+        <v>347</v>
+      </c>
+      <c r="C175" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A176" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="B176" t="s">
+        <v>348</v>
+      </c>
+      <c r="C176" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A177" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B177" t="s">
+        <v>349</v>
+      </c>
+      <c r="C177" t="s">
         <v>85</v>
       </c>
     </row>
@@ -3016,14 +3526,24 @@
     <hyperlink ref="A146" r:id="rId18"/>
     <hyperlink ref="A147" r:id="rId19"/>
     <hyperlink ref="A148" r:id="rId20"/>
+    <hyperlink ref="A149" r:id="rId21"/>
+    <hyperlink ref="A150" r:id="rId22"/>
+    <hyperlink ref="A151" r:id="rId23"/>
+    <hyperlink ref="A152" r:id="rId24"/>
+    <hyperlink ref="A165" r:id="rId25"/>
+    <hyperlink ref="A168" r:id="rId26"/>
+    <hyperlink ref="A169" r:id="rId27"/>
+    <hyperlink ref="A170" r:id="rId28"/>
+    <hyperlink ref="A171" r:id="rId29"/>
+    <hyperlink ref="A172" r:id="rId30"/>
+    <hyperlink ref="A173" r:id="rId31"/>
+    <hyperlink ref="A174" r:id="rId32"/>
+    <hyperlink ref="A175" r:id="rId33"/>
+    <hyperlink ref="A176" r:id="rId34"/>
+    <hyperlink ref="A177" r:id="rId35"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3033,14 +3553,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3050,13 +3565,8 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
OBI imports of value specifications, medical history (issue #46) and eligibility criteria (issue #45) for NCI BBRB
</commit_message>
<xml_diff>
--- a/src/external/ontoDog_input/ontoDog_input.xlsx
+++ b/src/external/ontoDog_input/ontoDog_input.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26606"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28908"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-26000" yWindow="6980" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="-35460" yWindow="3860" windowWidth="32880" windowHeight="18400"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,9 @@
   </sheets>
   <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="542">
   <si>
     <t>Homo sapiens</t>
   </si>
@@ -856,12 +859,6 @@
     <t>http://purl.obolibrary.org/obo/UO_0000005</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/UO_0000027</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/UO_0000196</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/OBI_0000835</t>
   </si>
   <si>
@@ -892,12 +889,6 @@
     <t>temperature unit</t>
   </si>
   <si>
-    <t>degree celsius</t>
-  </si>
-  <si>
-    <t>pH</t>
-  </si>
-  <si>
     <t>manufacturer</t>
   </si>
   <si>
@@ -958,12 +949,6 @@
     <t>http://purl.obolibrary.org/obo/OBI_0000947</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/UO_0000195</t>
-  </si>
-  <si>
-    <t>degree Fahrenheit</t>
-  </si>
-  <si>
     <t>RNA Integrity Number calculation</t>
   </si>
   <si>
@@ -1106,13 +1091,577 @@
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/OBI_0002554</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/IAO_0000144</t>
+  </si>
+  <si>
+    <t>conclusion textual entity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002190 </t>
+  </si>
+  <si>
+    <t>courier organization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002191 </t>
+  </si>
+  <si>
+    <t>courier tracking number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002192 </t>
+  </si>
+  <si>
+    <t>Leica Peloris rapid tissue processor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002194 </t>
+  </si>
+  <si>
+    <t>Microm Ergostar HM200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002195 </t>
+  </si>
+  <si>
+    <t>microtome blade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002196 </t>
+  </si>
+  <si>
+    <t>Sakura Low profile Accu-Edge microtome blade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002197 </t>
+  </si>
+  <si>
+    <t>tissue section thickness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002198 </t>
+  </si>
+  <si>
+    <t>molecular analysis facility organization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002199 </t>
+  </si>
+  <si>
+    <t>reason for lack of data item</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002200 </t>
+  </si>
+  <si>
+    <t>cannot be assessed determination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002201 </t>
+  </si>
+  <si>
+    <t>determination if assay will provide reliable results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002202 </t>
+  </si>
+  <si>
+    <t>GX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002203 </t>
+  </si>
+  <si>
+    <t>pTX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002204 </t>
+  </si>
+  <si>
+    <t>pNX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002205 </t>
+  </si>
+  <si>
+    <t>histologic grade according to AJCC 7th edition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002210 </t>
+  </si>
+  <si>
+    <t>histologic grade according to the Fuhrman Nuclear Grading System</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002215 </t>
+  </si>
+  <si>
+    <t>histologic grade for ovarian tumor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002216 </t>
+  </si>
+  <si>
+    <t>histologic grade for ovarian tumor according to a two-tier grading system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002219 </t>
+  </si>
+  <si>
+    <t>histologic grade for ovarian tumor according to the World Health Organization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002224 </t>
+  </si>
+  <si>
+    <t>pathologic primary tumor stage for colon and rectum according to AJCC 7th edition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002232 </t>
+  </si>
+  <si>
+    <t>pathologic primary tumor stage for lung according to AJCC 7th edition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002243 </t>
+  </si>
+  <si>
+    <t>pathologic primary tumor stage for kidney according to AJCC 7th edition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002256 </t>
+  </si>
+  <si>
+    <t>pathologic primary tumor stage for ovary according to AJCC 7th edition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002270 </t>
+  </si>
+  <si>
+    <t>pathologic lymph node stage for colon and rectum according to AJCC 7th edition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002279 </t>
+  </si>
+  <si>
+    <t>pathologic lymph node stage for lung according to AJCC 7th edition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002284 </t>
+  </si>
+  <si>
+    <t>pathologic lymph node stage for kidney according to AJCC 7th edition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002287 </t>
+  </si>
+  <si>
+    <t>pathologic lymph node stage for ovary according to AJCC 7th edition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002290 </t>
+  </si>
+  <si>
+    <t>pathologic distant metastases stage for colon according to AJCC 7th edition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002298 </t>
+  </si>
+  <si>
+    <t>pathologic distant metastases stage for lung according to AJCC 7th edition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002306 </t>
+  </si>
+  <si>
+    <t>pathologic distant metastases stage for kidney according to AJCC 7th edition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002310 </t>
+  </si>
+  <si>
+    <t>pathologic distant metastases stage for ovary according to AJCC 7th edition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002314 </t>
+  </si>
+  <si>
+    <t>clinical tumor stage group according to AJCC 7th edition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002326 </t>
+  </si>
+  <si>
+    <t>International Federation of Gynecology and Obstetrics cervical cancer stage value specification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002341 </t>
+  </si>
+  <si>
+    <t>International Federation of Gynecology and Obstetrics ovarian cancer stage value specification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002356 </t>
+  </si>
+  <si>
+    <t>performance status value specification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002357 </t>
+  </si>
+  <si>
+    <t>Eastern Cooperative Oncology Group score value specification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002363 </t>
+  </si>
+  <si>
+    <t>Karnofsky score vaue specification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002368 </t>
+  </si>
+  <si>
+    <t>clinical history of cancer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002369 </t>
+  </si>
+  <si>
+    <t>clinical history devoid of cancer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002370 </t>
+  </si>
+  <si>
+    <t>unknown clinical history of cancer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002371 </t>
+  </si>
+  <si>
+    <t>diagnosis of cancer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002372 </t>
+  </si>
+  <si>
+    <t>family clinical history of cancer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002373 </t>
+  </si>
+  <si>
+    <t>aunt clinical history of cancer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002374 </t>
+  </si>
+  <si>
+    <t>brother clinical history of cancer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002375 </t>
+  </si>
+  <si>
+    <t>daughter clinical history of cancer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002376 </t>
+  </si>
+  <si>
+    <t>father clinical history of cancer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002377 </t>
+  </si>
+  <si>
+    <t>mother clinical history of cancer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002378 </t>
+  </si>
+  <si>
+    <t>sister clinical history of cancer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002379 </t>
+  </si>
+  <si>
+    <t>son clinical history of cancer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002380 </t>
+  </si>
+  <si>
+    <t>uncle clinical history of cancer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002381 </t>
+  </si>
+  <si>
+    <t>grandmother clinical history of cancer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002382 </t>
+  </si>
+  <si>
+    <t>grandfather clinical history of cancer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002383 </t>
+  </si>
+  <si>
+    <t>nephew clinical history of cancer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002384 </t>
+  </si>
+  <si>
+    <t>niece clinical history of cancer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002385 </t>
+  </si>
+  <si>
+    <t>diagnosis of infectious disease</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002386 </t>
+  </si>
+  <si>
+    <t>diagnosis of hepatitis B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002387 </t>
+  </si>
+  <si>
+    <t>diagnosis of hepatitis C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002388 </t>
+  </si>
+  <si>
+    <t>diagnosis of HIV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002389 </t>
+  </si>
+  <si>
+    <t>clinical history of repeated HIV assays</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002390 </t>
+  </si>
+  <si>
+    <t>exposure to second hand smoke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002391 </t>
+  </si>
+  <si>
+    <t>exposure to second hand smoke in household during childhood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002392 </t>
+  </si>
+  <si>
+    <t>exposure to second hand smoke in current household</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002393 </t>
+  </si>
+  <si>
+    <t>pregnancy history</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002394 </t>
+  </si>
+  <si>
+    <t>number of pregnancies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002395 </t>
+  </si>
+  <si>
+    <t>number of live births</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002396 </t>
+  </si>
+  <si>
+    <t>age when gave birth to first child</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002397 </t>
+  </si>
+  <si>
+    <t>gynecologic surgery history</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002398 </t>
+  </si>
+  <si>
+    <t>hysterectomy history</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002399 </t>
+  </si>
+  <si>
+    <t>unilateral oophorectomy history</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002400 </t>
+  </si>
+  <si>
+    <t>neither hysterectomy nor oophorectomy history</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002401 </t>
+  </si>
+  <si>
+    <t>hormonal birth control use history</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002402 </t>
+  </si>
+  <si>
+    <t>hormonal birth control former use history</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002403 </t>
+  </si>
+  <si>
+    <t>hormonal birth control current use history</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002404 </t>
+  </si>
+  <si>
+    <t>no hormonal birth control use history</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002405 </t>
+  </si>
+  <si>
+    <t>hormonal replacement therapy history</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002406 </t>
+  </si>
+  <si>
+    <t>delivery form for hormonal replacement therapy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002407 </t>
+  </si>
+  <si>
+    <t>pill delivery form for hormonal replacement therapy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002408 </t>
+  </si>
+  <si>
+    <t>patch delivery form for hormonal replacement therapy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002409 </t>
+  </si>
+  <si>
+    <t>cream delivery form for hormonal replacement therapy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002410 </t>
+  </si>
+  <si>
+    <t>menopausal status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002411 </t>
+  </si>
+  <si>
+    <t>indeterminate menopausal status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002412 </t>
+  </si>
+  <si>
+    <t>premenopausal status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002413 </t>
+  </si>
+  <si>
+    <t>perimenopausal status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002414 </t>
+  </si>
+  <si>
+    <t>postmenopausal status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002415 </t>
+  </si>
+  <si>
+    <t>exposure to environmental and workplace carcinogens history</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002416 </t>
+  </si>
+  <si>
+    <t>exposure to arsenic history</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002417 </t>
+  </si>
+  <si>
+    <t>exposure to asbestos history</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002418 </t>
+  </si>
+  <si>
+    <t>exposure to diesel exhaust history</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002419 </t>
+  </si>
+  <si>
+    <t>exposure to chromium history</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002420 </t>
+  </si>
+  <si>
+    <t>exposure to silica history</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002421 </t>
+  </si>
+  <si>
+    <t>indicator of whether an inclusion criterion was met</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/OBI_0002422 </t>
+  </si>
+  <si>
+    <t>indicator of whether all inclusion criteria were met</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000051</t>
+  </si>
+  <si>
+    <t>concentration unit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1162,6 +1711,11 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="-webkit-standard"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1189,7 +1743,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1205,6 +1759,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
@@ -1515,10 +2070,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E177"/>
+  <dimension ref="A1:E268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A155" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A178" sqref="A178"/>
+    <sheetView tabSelected="1" topLeftCell="A245" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C268" sqref="C268"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2997,7 +3552,7 @@
         <v>268</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C132" t="s">
         <v>85</v>
@@ -3008,7 +3563,7 @@
         <v>269</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C133" t="s">
         <v>85</v>
@@ -3019,7 +3574,7 @@
         <v>270</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C134" t="s">
         <v>85</v>
@@ -3030,7 +3585,7 @@
         <v>271</v>
       </c>
       <c r="B135" s="5" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C135" t="s">
         <v>85</v>
@@ -3041,7 +3596,7 @@
         <v>272</v>
       </c>
       <c r="B136" s="5" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C136" t="s">
         <v>85</v>
@@ -3052,7 +3607,7 @@
         <v>273</v>
       </c>
       <c r="B137" s="5" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C137" t="s">
         <v>85</v>
@@ -3063,7 +3618,7 @@
         <v>274</v>
       </c>
       <c r="B138" s="5" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C138" t="s">
         <v>85</v>
@@ -3074,7 +3629,7 @@
         <v>275</v>
       </c>
       <c r="B139" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C139" t="s">
         <v>85</v>
@@ -3085,7 +3640,7 @@
         <v>276</v>
       </c>
       <c r="B140" s="6" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C140" t="s">
         <v>85</v>
@@ -3096,26 +3651,26 @@
         <v>277</v>
       </c>
       <c r="B141" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="C141" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A142" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B142" s="6" t="s">
         <v>289</v>
       </c>
-      <c r="C141" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A142" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="B142" s="6" t="s">
+      <c r="C142" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
         <v>290</v>
-      </c>
-      <c r="C142" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A143" s="3" t="s">
-        <v>279</v>
       </c>
       <c r="B143" s="6" t="s">
         <v>291</v>
@@ -3136,11 +3691,11 @@
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A145" t="s">
+      <c r="A145" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B145" s="6" t="s">
         <v>294</v>
-      </c>
-      <c r="B145" s="6" t="s">
-        <v>295</v>
       </c>
       <c r="C145" t="s">
         <v>85</v>
@@ -3148,10 +3703,10 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B146" s="6" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C146" t="s">
         <v>85</v>
@@ -3159,9 +3714,9 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="B147" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="B147" s="7" t="s">
         <v>298</v>
       </c>
       <c r="C147" t="s">
@@ -3170,9 +3725,9 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="B148" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="B148" s="7" t="s">
         <v>299</v>
       </c>
       <c r="C148" t="s">
@@ -3181,10 +3736,10 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B149" s="7" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C149" t="s">
         <v>85</v>
@@ -3192,32 +3747,32 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="B150" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="C150" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
         <v>307</v>
       </c>
-      <c r="B150" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="C150" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A151" s="1" t="s">
+      <c r="B151" t="s">
+        <v>306</v>
+      </c>
+      <c r="C151" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
         <v>308</v>
       </c>
-      <c r="B151" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="C151" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A152" s="1" t="s">
+      <c r="B152" t="s">
         <v>309</v>
-      </c>
-      <c r="B152" s="7" t="s">
-        <v>305</v>
       </c>
       <c r="C152" t="s">
         <v>85</v>
@@ -3228,15 +3783,18 @@
         <v>310</v>
       </c>
       <c r="B153" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C153" t="s">
         <v>85</v>
+      </c>
+      <c r="E153" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B154" t="s">
         <v>312</v>
@@ -3247,10 +3805,10 @@
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
+        <v>315</v>
+      </c>
+      <c r="B155" t="s">
         <v>314</v>
-      </c>
-      <c r="B155" t="s">
-        <v>315</v>
       </c>
       <c r="C155" t="s">
         <v>85</v>
@@ -3260,19 +3818,16 @@
       <c r="A156" t="s">
         <v>316</v>
       </c>
-      <c r="B156" t="s">
-        <v>319</v>
+      <c r="B156" s="8" t="s">
+        <v>317</v>
       </c>
       <c r="C156" t="s">
         <v>85</v>
-      </c>
-      <c r="E156" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B157" t="s">
         <v>318</v>
@@ -3283,10 +3838,10 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
+        <v>320</v>
+      </c>
+      <c r="B158" t="s">
         <v>321</v>
-      </c>
-      <c r="B158" t="s">
-        <v>320</v>
       </c>
       <c r="C158" t="s">
         <v>85</v>
@@ -3294,10 +3849,10 @@
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
+        <v>323</v>
+      </c>
+      <c r="B159" t="s">
         <v>322</v>
-      </c>
-      <c r="B159" s="8" t="s">
-        <v>323</v>
       </c>
       <c r="C159" t="s">
         <v>85</v>
@@ -3305,10 +3860,10 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
+        <v>324</v>
+      </c>
+      <c r="B160" t="s">
         <v>325</v>
-      </c>
-      <c r="B160" t="s">
-        <v>324</v>
       </c>
       <c r="C160" t="s">
         <v>85</v>
@@ -3326,11 +3881,11 @@
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A162" t="s">
+      <c r="A162" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="B162" t="s">
         <v>329</v>
-      </c>
-      <c r="B162" t="s">
-        <v>328</v>
       </c>
       <c r="C162" t="s">
         <v>85</v>
@@ -3349,10 +3904,10 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
+        <v>333</v>
+      </c>
+      <c r="B164" t="s">
         <v>332</v>
-      </c>
-      <c r="B164" t="s">
-        <v>333</v>
       </c>
       <c r="C164" t="s">
         <v>85</v>
@@ -3360,32 +3915,32 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B165" t="s">
         <v>334</v>
       </c>
-      <c r="B165" t="s">
+      <c r="C165" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A166" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B166" t="s">
         <v>335</v>
       </c>
-      <c r="C165" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A166" t="s">
+      <c r="C166" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A167" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="B167" t="s">
         <v>336</v>
-      </c>
-      <c r="B166" t="s">
-        <v>337</v>
-      </c>
-      <c r="C166" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A167" t="s">
-        <v>339</v>
-      </c>
-      <c r="B167" t="s">
-        <v>338</v>
       </c>
       <c r="C167" t="s">
         <v>85</v>
@@ -3393,10 +3948,10 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="B168" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C168" t="s">
         <v>85</v>
@@ -3404,10 +3959,10 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B169" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C169" t="s">
         <v>85</v>
@@ -3415,10 +3970,10 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="B170" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C170" t="s">
         <v>85</v>
@@ -3426,10 +3981,10 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="B171" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="C171" t="s">
         <v>85</v>
@@ -3437,10 +3992,10 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="B172" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C172" t="s">
         <v>85</v>
@@ -3448,10 +4003,10 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="B173" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C173" t="s">
         <v>85</v>
@@ -3459,45 +4014,1046 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B174" t="s">
+        <v>343</v>
+      </c>
+      <c r="C174" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>354</v>
+      </c>
+      <c r="B175" t="s">
+        <v>355</v>
+      </c>
+      <c r="C175" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A176" s="9" t="s">
         <v>356</v>
       </c>
-      <c r="B174" t="s">
-        <v>346</v>
-      </c>
-      <c r="C174" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A175" s="1" t="s">
+      <c r="B176" t="s">
         <v>357</v>
       </c>
-      <c r="B175" t="s">
-        <v>347</v>
-      </c>
-      <c r="C175" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A176" s="1" t="s">
+      <c r="C176" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A177" s="9" t="s">
         <v>358</v>
       </c>
-      <c r="B176" t="s">
-        <v>348</v>
-      </c>
-      <c r="C176" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A177" s="1" t="s">
+      <c r="B177" t="s">
         <v>359</v>
       </c>
-      <c r="B177" t="s">
-        <v>349</v>
-      </c>
       <c r="C177" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A178" s="9" t="s">
+        <v>360</v>
+      </c>
+      <c r="B178" t="s">
+        <v>361</v>
+      </c>
+      <c r="C178" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A179" s="9" t="s">
+        <v>362</v>
+      </c>
+      <c r="B179" t="s">
+        <v>363</v>
+      </c>
+      <c r="C179" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A180" s="9" t="s">
+        <v>364</v>
+      </c>
+      <c r="B180" t="s">
+        <v>365</v>
+      </c>
+      <c r="C180" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A181" s="9" t="s">
+        <v>366</v>
+      </c>
+      <c r="B181" t="s">
+        <v>367</v>
+      </c>
+      <c r="C181" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A182" s="9" t="s">
+        <v>368</v>
+      </c>
+      <c r="B182" t="s">
+        <v>369</v>
+      </c>
+      <c r="C182" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A183" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="B183" t="s">
+        <v>371</v>
+      </c>
+      <c r="C183" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A184" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="B184" t="s">
+        <v>373</v>
+      </c>
+      <c r="C184" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A185" s="9" t="s">
+        <v>374</v>
+      </c>
+      <c r="B185" t="s">
+        <v>375</v>
+      </c>
+      <c r="C185" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A186" s="9" t="s">
+        <v>376</v>
+      </c>
+      <c r="B186" t="s">
+        <v>377</v>
+      </c>
+      <c r="C186" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A187" s="9" t="s">
+        <v>378</v>
+      </c>
+      <c r="B187" t="s">
+        <v>379</v>
+      </c>
+      <c r="C187" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A188" s="9" t="s">
+        <v>380</v>
+      </c>
+      <c r="B188" t="s">
+        <v>381</v>
+      </c>
+      <c r="C188" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A189" s="9" t="s">
+        <v>382</v>
+      </c>
+      <c r="B189" t="s">
+        <v>383</v>
+      </c>
+      <c r="C189" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A190" s="9" t="s">
+        <v>384</v>
+      </c>
+      <c r="B190" t="s">
+        <v>385</v>
+      </c>
+      <c r="C190" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A191" s="9" t="s">
+        <v>386</v>
+      </c>
+      <c r="B191" t="s">
+        <v>387</v>
+      </c>
+      <c r="C191" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A192" s="9" t="s">
+        <v>388</v>
+      </c>
+      <c r="B192" t="s">
+        <v>389</v>
+      </c>
+      <c r="C192" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A193" s="9" t="s">
+        <v>390</v>
+      </c>
+      <c r="B193" t="s">
+        <v>391</v>
+      </c>
+      <c r="C193" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A194" s="9" t="s">
+        <v>392</v>
+      </c>
+      <c r="B194" t="s">
+        <v>393</v>
+      </c>
+      <c r="C194" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A195" s="9" t="s">
+        <v>394</v>
+      </c>
+      <c r="B195" t="s">
+        <v>395</v>
+      </c>
+      <c r="C195" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A196" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="B196" t="s">
+        <v>397</v>
+      </c>
+      <c r="C196" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A197" s="9" t="s">
+        <v>398</v>
+      </c>
+      <c r="B197" t="s">
+        <v>399</v>
+      </c>
+      <c r="C197" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A198" s="9" t="s">
+        <v>400</v>
+      </c>
+      <c r="B198" t="s">
+        <v>401</v>
+      </c>
+      <c r="C198" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A199" s="9" t="s">
+        <v>402</v>
+      </c>
+      <c r="B199" t="s">
+        <v>403</v>
+      </c>
+      <c r="C199" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A200" s="9" t="s">
+        <v>404</v>
+      </c>
+      <c r="B200" t="s">
+        <v>405</v>
+      </c>
+      <c r="C200" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A201" s="9" t="s">
+        <v>406</v>
+      </c>
+      <c r="B201" t="s">
+        <v>407</v>
+      </c>
+      <c r="C201" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A202" s="9" t="s">
+        <v>408</v>
+      </c>
+      <c r="B202" t="s">
+        <v>409</v>
+      </c>
+      <c r="C202" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A203" s="9" t="s">
+        <v>410</v>
+      </c>
+      <c r="B203" t="s">
+        <v>411</v>
+      </c>
+      <c r="C203" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A204" s="9" t="s">
+        <v>412</v>
+      </c>
+      <c r="B204" t="s">
+        <v>413</v>
+      </c>
+      <c r="C204" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A205" s="9" t="s">
+        <v>414</v>
+      </c>
+      <c r="B205" t="s">
+        <v>415</v>
+      </c>
+      <c r="C205" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A206" s="9" t="s">
+        <v>416</v>
+      </c>
+      <c r="B206" t="s">
+        <v>417</v>
+      </c>
+      <c r="C206" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A207" s="9" t="s">
+        <v>418</v>
+      </c>
+      <c r="B207" t="s">
+        <v>419</v>
+      </c>
+      <c r="C207" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A208" s="9" t="s">
+        <v>420</v>
+      </c>
+      <c r="B208" t="s">
+        <v>421</v>
+      </c>
+      <c r="C208" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A209" s="9" t="s">
+        <v>422</v>
+      </c>
+      <c r="B209" t="s">
+        <v>423</v>
+      </c>
+      <c r="C209" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A210" s="9" t="s">
+        <v>424</v>
+      </c>
+      <c r="B210" t="s">
+        <v>425</v>
+      </c>
+      <c r="C210" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A211" s="9" t="s">
+        <v>426</v>
+      </c>
+      <c r="B211" t="s">
+        <v>427</v>
+      </c>
+      <c r="C211" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A212" s="9" t="s">
+        <v>428</v>
+      </c>
+      <c r="B212" t="s">
+        <v>429</v>
+      </c>
+      <c r="C212" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A213" s="9" t="s">
+        <v>430</v>
+      </c>
+      <c r="B213" t="s">
+        <v>431</v>
+      </c>
+      <c r="C213" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A214" s="9" t="s">
+        <v>432</v>
+      </c>
+      <c r="B214" t="s">
+        <v>433</v>
+      </c>
+      <c r="C214" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A215" s="9" t="s">
+        <v>434</v>
+      </c>
+      <c r="B215" t="s">
+        <v>435</v>
+      </c>
+      <c r="C215" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A216" s="9" t="s">
+        <v>436</v>
+      </c>
+      <c r="B216" t="s">
+        <v>437</v>
+      </c>
+      <c r="C216" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A217" s="9" t="s">
+        <v>438</v>
+      </c>
+      <c r="B217" t="s">
+        <v>439</v>
+      </c>
+      <c r="C217" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A218" s="9" t="s">
+        <v>440</v>
+      </c>
+      <c r="B218" t="s">
+        <v>441</v>
+      </c>
+      <c r="C218" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A219" s="9" t="s">
+        <v>442</v>
+      </c>
+      <c r="B219" t="s">
+        <v>443</v>
+      </c>
+      <c r="C219" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A220" s="9" t="s">
+        <v>444</v>
+      </c>
+      <c r="B220" t="s">
+        <v>445</v>
+      </c>
+      <c r="C220" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A221" s="9" t="s">
+        <v>446</v>
+      </c>
+      <c r="B221" t="s">
+        <v>447</v>
+      </c>
+      <c r="C221" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A222" s="9" t="s">
+        <v>448</v>
+      </c>
+      <c r="B222" t="s">
+        <v>449</v>
+      </c>
+      <c r="C222" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A223" s="9" t="s">
+        <v>450</v>
+      </c>
+      <c r="B223" t="s">
+        <v>451</v>
+      </c>
+      <c r="C223" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A224" s="9" t="s">
+        <v>452</v>
+      </c>
+      <c r="B224" t="s">
+        <v>453</v>
+      </c>
+      <c r="C224" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A225" s="9" t="s">
+        <v>454</v>
+      </c>
+      <c r="B225" t="s">
+        <v>455</v>
+      </c>
+      <c r="C225" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A226" s="9" t="s">
+        <v>456</v>
+      </c>
+      <c r="B226" t="s">
+        <v>457</v>
+      </c>
+      <c r="C226" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A227" s="9" t="s">
+        <v>458</v>
+      </c>
+      <c r="B227" t="s">
+        <v>459</v>
+      </c>
+      <c r="C227" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A228" s="9" t="s">
+        <v>460</v>
+      </c>
+      <c r="B228" t="s">
+        <v>461</v>
+      </c>
+      <c r="C228" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A229" s="9" t="s">
+        <v>462</v>
+      </c>
+      <c r="B229" t="s">
+        <v>463</v>
+      </c>
+      <c r="C229" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A230" s="9" t="s">
+        <v>464</v>
+      </c>
+      <c r="B230" t="s">
+        <v>465</v>
+      </c>
+      <c r="C230" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A231" s="9" t="s">
+        <v>466</v>
+      </c>
+      <c r="B231" t="s">
+        <v>467</v>
+      </c>
+      <c r="C231" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A232" s="9" t="s">
+        <v>468</v>
+      </c>
+      <c r="B232" t="s">
+        <v>469</v>
+      </c>
+      <c r="C232" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A233" s="9" t="s">
+        <v>470</v>
+      </c>
+      <c r="B233" t="s">
+        <v>471</v>
+      </c>
+      <c r="C233" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A234" s="9" t="s">
+        <v>472</v>
+      </c>
+      <c r="B234" t="s">
+        <v>473</v>
+      </c>
+      <c r="C234" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A235" s="9" t="s">
+        <v>474</v>
+      </c>
+      <c r="B235" t="s">
+        <v>475</v>
+      </c>
+      <c r="C235" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A236" s="9" t="s">
+        <v>476</v>
+      </c>
+      <c r="B236" t="s">
+        <v>477</v>
+      </c>
+      <c r="C236" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A237" s="9" t="s">
+        <v>478</v>
+      </c>
+      <c r="B237" t="s">
+        <v>479</v>
+      </c>
+      <c r="C237" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A238" s="9" t="s">
+        <v>480</v>
+      </c>
+      <c r="B238" t="s">
+        <v>481</v>
+      </c>
+      <c r="C238" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A239" s="9" t="s">
+        <v>482</v>
+      </c>
+      <c r="B239" t="s">
+        <v>483</v>
+      </c>
+      <c r="C239" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A240" s="9" t="s">
+        <v>484</v>
+      </c>
+      <c r="B240" t="s">
+        <v>485</v>
+      </c>
+      <c r="C240" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A241" s="9" t="s">
+        <v>486</v>
+      </c>
+      <c r="B241" t="s">
+        <v>487</v>
+      </c>
+      <c r="C241" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A242" s="9" t="s">
+        <v>488</v>
+      </c>
+      <c r="B242" t="s">
+        <v>489</v>
+      </c>
+      <c r="C242" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A243" s="9" t="s">
+        <v>490</v>
+      </c>
+      <c r="B243" t="s">
+        <v>491</v>
+      </c>
+      <c r="C243" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A244" s="9" t="s">
+        <v>492</v>
+      </c>
+      <c r="B244" t="s">
+        <v>493</v>
+      </c>
+      <c r="C244" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A245" s="9" t="s">
+        <v>494</v>
+      </c>
+      <c r="B245" t="s">
+        <v>495</v>
+      </c>
+      <c r="C245" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A246" s="9" t="s">
+        <v>496</v>
+      </c>
+      <c r="B246" t="s">
+        <v>497</v>
+      </c>
+      <c r="C246" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A247" s="9" t="s">
+        <v>498</v>
+      </c>
+      <c r="B247" t="s">
+        <v>499</v>
+      </c>
+      <c r="C247" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A248" s="9" t="s">
+        <v>500</v>
+      </c>
+      <c r="B248" t="s">
+        <v>501</v>
+      </c>
+      <c r="C248" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A249" s="9" t="s">
+        <v>502</v>
+      </c>
+      <c r="B249" t="s">
+        <v>503</v>
+      </c>
+      <c r="C249" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A250" s="9" t="s">
+        <v>504</v>
+      </c>
+      <c r="B250" t="s">
+        <v>505</v>
+      </c>
+      <c r="C250" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A251" s="9" t="s">
+        <v>506</v>
+      </c>
+      <c r="B251" t="s">
+        <v>507</v>
+      </c>
+      <c r="C251" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A252" s="9" t="s">
+        <v>508</v>
+      </c>
+      <c r="B252" t="s">
+        <v>509</v>
+      </c>
+      <c r="C252" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A253" s="9" t="s">
+        <v>510</v>
+      </c>
+      <c r="B253" t="s">
+        <v>511</v>
+      </c>
+      <c r="C253" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A254" s="9" t="s">
+        <v>512</v>
+      </c>
+      <c r="B254" t="s">
+        <v>513</v>
+      </c>
+      <c r="C254" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A255" s="9" t="s">
+        <v>514</v>
+      </c>
+      <c r="B255" t="s">
+        <v>515</v>
+      </c>
+      <c r="C255" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A256" s="9" t="s">
+        <v>516</v>
+      </c>
+      <c r="B256" t="s">
+        <v>517</v>
+      </c>
+      <c r="C256" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A257" s="9" t="s">
+        <v>518</v>
+      </c>
+      <c r="B257" t="s">
+        <v>519</v>
+      </c>
+      <c r="C257" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A258" s="9" t="s">
+        <v>520</v>
+      </c>
+      <c r="B258" t="s">
+        <v>521</v>
+      </c>
+      <c r="C258" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A259" s="9" t="s">
+        <v>522</v>
+      </c>
+      <c r="B259" t="s">
+        <v>523</v>
+      </c>
+      <c r="C259" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A260" s="9" t="s">
+        <v>524</v>
+      </c>
+      <c r="B260" t="s">
+        <v>525</v>
+      </c>
+      <c r="C260" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A261" s="9" t="s">
+        <v>526</v>
+      </c>
+      <c r="B261" t="s">
+        <v>527</v>
+      </c>
+      <c r="C261" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A262" s="9" t="s">
+        <v>528</v>
+      </c>
+      <c r="B262" t="s">
+        <v>529</v>
+      </c>
+      <c r="C262" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A263" s="9" t="s">
+        <v>530</v>
+      </c>
+      <c r="B263" t="s">
+        <v>531</v>
+      </c>
+      <c r="C263" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A264" s="9" t="s">
+        <v>532</v>
+      </c>
+      <c r="B264" t="s">
+        <v>533</v>
+      </c>
+      <c r="C264" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A265" s="9" t="s">
+        <v>534</v>
+      </c>
+      <c r="B265" t="s">
+        <v>535</v>
+      </c>
+      <c r="C265" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A266" s="9" t="s">
+        <v>536</v>
+      </c>
+      <c r="B266" t="s">
+        <v>537</v>
+      </c>
+      <c r="C266" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A267" s="9" t="s">
+        <v>538</v>
+      </c>
+      <c r="B267" t="s">
+        <v>539</v>
+      </c>
+      <c r="C267" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A268" t="s">
+        <v>540</v>
+      </c>
+      <c r="B268" t="s">
+        <v>541</v>
+      </c>
+      <c r="C268" t="s">
         <v>85</v>
       </c>
     </row>
@@ -3521,26 +5077,24 @@
     <hyperlink ref="A140" r:id="rId13"/>
     <hyperlink ref="A141" r:id="rId14"/>
     <hyperlink ref="A142" r:id="rId15"/>
-    <hyperlink ref="A143" r:id="rId16"/>
-    <hyperlink ref="A144" r:id="rId17"/>
+    <hyperlink ref="A144" r:id="rId16"/>
+    <hyperlink ref="A145" r:id="rId17"/>
     <hyperlink ref="A146" r:id="rId18"/>
     <hyperlink ref="A147" r:id="rId19"/>
     <hyperlink ref="A148" r:id="rId20"/>
     <hyperlink ref="A149" r:id="rId21"/>
     <hyperlink ref="A150" r:id="rId22"/>
-    <hyperlink ref="A151" r:id="rId23"/>
-    <hyperlink ref="A152" r:id="rId24"/>
-    <hyperlink ref="A165" r:id="rId25"/>
-    <hyperlink ref="A168" r:id="rId26"/>
-    <hyperlink ref="A169" r:id="rId27"/>
-    <hyperlink ref="A170" r:id="rId28"/>
-    <hyperlink ref="A171" r:id="rId29"/>
-    <hyperlink ref="A172" r:id="rId30"/>
-    <hyperlink ref="A173" r:id="rId31"/>
-    <hyperlink ref="A174" r:id="rId32"/>
-    <hyperlink ref="A175" r:id="rId33"/>
-    <hyperlink ref="A176" r:id="rId34"/>
-    <hyperlink ref="A177" r:id="rId35"/>
+    <hyperlink ref="A162" r:id="rId23"/>
+    <hyperlink ref="A165" r:id="rId24"/>
+    <hyperlink ref="A166" r:id="rId25"/>
+    <hyperlink ref="A167" r:id="rId26"/>
+    <hyperlink ref="A168" r:id="rId27"/>
+    <hyperlink ref="A169" r:id="rId28"/>
+    <hyperlink ref="A170" r:id="rId29"/>
+    <hyperlink ref="A171" r:id="rId30"/>
+    <hyperlink ref="A172" r:id="rId31"/>
+    <hyperlink ref="A173" r:id="rId32"/>
+    <hyperlink ref="A174" r:id="rId33"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
addd time unit explicitly to get unit instances as per issue #54
</commit_message>
<xml_diff>
--- a/src/external/ontoDog_input/ontoDog_input.xlsx
+++ b/src/external/ontoDog_input/ontoDog_input.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28908"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stoeckrtTM/Git/biobanking-ontology/ontology/src/external/ontoDog_input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stoeckrt/Git/biobanking/ontology/src/external/ontoDog_input/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E8E695-2701-3B46-A6F6-FCDD59A58970}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35460" yWindow="3860" windowWidth="32880" windowHeight="18400"/>
+    <workbookView xWindow="-35460" yWindow="3860" windowWidth="32880" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="544">
   <si>
     <t>Homo sapiens</t>
   </si>
@@ -1655,13 +1656,19 @@
   </si>
   <si>
     <t>concentration unit</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000003</t>
+  </si>
+  <si>
+    <t>time unit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2069,14 +2076,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E268"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E269"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A245" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C268" sqref="C268"/>
+    <sheetView tabSelected="1" topLeftCell="A261" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D273" sqref="D273"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="57" customWidth="1"/>
     <col min="2" max="2" width="49.1640625" customWidth="1"/>
@@ -2085,7 +2092,7 @@
     <col min="5" max="5" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>79</v>
       </c>
@@ -2102,7 +2109,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -2113,7 +2120,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>95</v>
       </c>
@@ -2124,7 +2131,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2135,7 +2142,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -2146,7 +2153,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -2157,7 +2164,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -2168,7 +2175,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -2179,7 +2186,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -2190,7 +2197,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -2201,7 +2208,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -2212,7 +2219,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>101</v>
       </c>
@@ -2226,7 +2233,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -2237,7 +2244,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -2248,7 +2255,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -2259,7 +2266,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>86</v>
       </c>
@@ -2273,7 +2280,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -2284,7 +2291,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -2295,7 +2302,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>88</v>
       </c>
@@ -2306,7 +2313,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -2317,7 +2324,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -2328,7 +2335,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -2339,7 +2346,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -2350,7 +2357,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -2361,7 +2368,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>44</v>
       </c>
@@ -2372,7 +2379,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -2383,7 +2390,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -2394,7 +2401,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>48</v>
       </c>
@@ -2405,7 +2412,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -2416,7 +2423,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
         <v>52</v>
       </c>
@@ -2427,7 +2434,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
         <v>103</v>
       </c>
@@ -2438,7 +2445,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
         <v>50</v>
       </c>
@@ -2449,7 +2456,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>58</v>
       </c>
@@ -2460,7 +2467,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>54</v>
       </c>
@@ -2471,7 +2478,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>56</v>
       </c>
@@ -2482,7 +2489,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>60</v>
       </c>
@@ -2493,7 +2500,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>62</v>
       </c>
@@ -2504,7 +2511,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>89</v>
       </c>
@@ -2515,7 +2522,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>93</v>
       </c>
@@ -2526,7 +2533,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>72</v>
       </c>
@@ -2537,7 +2544,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>70</v>
       </c>
@@ -2548,7 +2555,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
         <v>98</v>
       </c>
@@ -2559,7 +2566,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
         <v>68</v>
       </c>
@@ -2573,7 +2580,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
         <v>64</v>
       </c>
@@ -2584,7 +2591,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
         <v>74</v>
       </c>
@@ -2595,7 +2602,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
         <v>66</v>
       </c>
@@ -2606,7 +2613,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5">
       <c r="A47" t="s">
         <v>92</v>
       </c>
@@ -2617,7 +2624,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5">
       <c r="A48" t="s">
         <v>97</v>
       </c>
@@ -2628,7 +2635,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
         <v>76</v>
       </c>
@@ -2639,7 +2646,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
         <v>78</v>
       </c>
@@ -2650,7 +2657,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5">
       <c r="A51" t="s">
         <v>105</v>
       </c>
@@ -2661,7 +2668,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5">
       <c r="A52" t="s">
         <v>108</v>
       </c>
@@ -2672,7 +2679,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5">
       <c r="A53" t="s">
         <v>109</v>
       </c>
@@ -2686,7 +2693,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5">
       <c r="A54" t="s">
         <v>111</v>
       </c>
@@ -2697,7 +2704,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5">
       <c r="A55" t="s">
         <v>160</v>
       </c>
@@ -2708,7 +2715,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5">
       <c r="A56" t="s">
         <v>161</v>
       </c>
@@ -2719,7 +2726,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5">
       <c r="A57" t="s">
         <v>162</v>
       </c>
@@ -2730,7 +2737,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5">
       <c r="A58" t="s">
         <v>163</v>
       </c>
@@ -2741,7 +2748,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5">
       <c r="A59" t="s">
         <v>164</v>
       </c>
@@ -2752,7 +2759,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5">
       <c r="A60" t="s">
         <v>165</v>
       </c>
@@ -2763,7 +2770,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5">
       <c r="A61" t="s">
         <v>166</v>
       </c>
@@ -2774,7 +2781,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5">
       <c r="A62" t="s">
         <v>169</v>
       </c>
@@ -2785,7 +2792,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5">
       <c r="A63" t="s">
         <v>170</v>
       </c>
@@ -2796,7 +2803,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5">
       <c r="A64" t="s">
         <v>171</v>
       </c>
@@ -2807,7 +2814,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3">
       <c r="A65" t="s">
         <v>172</v>
       </c>
@@ -2818,7 +2825,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3">
       <c r="A66" t="s">
         <v>173</v>
       </c>
@@ -2829,7 +2836,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3">
       <c r="A67" t="s">
         <v>174</v>
       </c>
@@ -2840,7 +2847,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3">
       <c r="A68" t="s">
         <v>175</v>
       </c>
@@ -2851,7 +2858,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3">
       <c r="A69" t="s">
         <v>176</v>
       </c>
@@ -2862,7 +2869,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3">
       <c r="A70" t="s">
         <v>177</v>
       </c>
@@ -2873,7 +2880,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3">
       <c r="A71" t="s">
         <v>178</v>
       </c>
@@ -2884,7 +2891,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3">
       <c r="A72" t="s">
         <v>179</v>
       </c>
@@ -2895,7 +2902,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3">
       <c r="A73" t="s">
         <v>180</v>
       </c>
@@ -2906,7 +2913,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3">
       <c r="A74" t="s">
         <v>181</v>
       </c>
@@ -2917,7 +2924,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3">
       <c r="A75" t="s">
         <v>182</v>
       </c>
@@ -2928,7 +2935,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3">
       <c r="A76" t="s">
         <v>183</v>
       </c>
@@ -2939,7 +2946,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3">
       <c r="A77" t="s">
         <v>184</v>
       </c>
@@ -2950,7 +2957,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3">
       <c r="A78" t="s">
         <v>185</v>
       </c>
@@ -2961,7 +2968,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3">
       <c r="A79" t="s">
         <v>186</v>
       </c>
@@ -2972,7 +2979,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3">
       <c r="A80" t="s">
         <v>187</v>
       </c>
@@ -2983,7 +2990,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3">
       <c r="A81" t="s">
         <v>188</v>
       </c>
@@ -2994,7 +3001,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3">
       <c r="A82" t="s">
         <v>189</v>
       </c>
@@ -3005,7 +3012,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3">
       <c r="A83" t="s">
         <v>190</v>
       </c>
@@ -3016,7 +3023,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3">
       <c r="A84" t="s">
         <v>191</v>
       </c>
@@ -3027,7 +3034,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3">
       <c r="A85" t="s">
         <v>192</v>
       </c>
@@ -3038,7 +3045,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3">
       <c r="A86" t="s">
         <v>193</v>
       </c>
@@ -3049,7 +3056,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3">
       <c r="A87" t="s">
         <v>194</v>
       </c>
@@ -3060,7 +3067,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3">
       <c r="A88" t="s">
         <v>195</v>
       </c>
@@ -3071,7 +3078,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3">
       <c r="A89" t="s">
         <v>196</v>
       </c>
@@ -3082,7 +3089,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3">
       <c r="A90" t="s">
         <v>197</v>
       </c>
@@ -3093,7 +3100,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3">
       <c r="A91" t="s">
         <v>198</v>
       </c>
@@ -3104,7 +3111,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3">
       <c r="A92" t="s">
         <v>199</v>
       </c>
@@ -3115,7 +3122,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3">
       <c r="A93" t="s">
         <v>200</v>
       </c>
@@ -3126,7 +3133,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3">
       <c r="A94" t="s">
         <v>201</v>
       </c>
@@ -3137,7 +3144,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3">
       <c r="A95" t="s">
         <v>202</v>
       </c>
@@ -3148,7 +3155,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3">
       <c r="A96" t="s">
         <v>203</v>
       </c>
@@ -3159,7 +3166,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3">
       <c r="A97" t="s">
         <v>204</v>
       </c>
@@ -3170,7 +3177,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3">
       <c r="A98" t="s">
         <v>205</v>
       </c>
@@ -3181,7 +3188,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3">
       <c r="A99" t="s">
         <v>206</v>
       </c>
@@ -3192,7 +3199,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3">
       <c r="A100" t="s">
         <v>168</v>
       </c>
@@ -3203,7 +3210,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3">
       <c r="A101" t="s">
         <v>167</v>
       </c>
@@ -3214,7 +3221,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3">
       <c r="A102" t="s">
         <v>207</v>
       </c>
@@ -3225,7 +3232,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3">
       <c r="A103" t="s">
         <v>210</v>
       </c>
@@ -3236,7 +3243,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3">
       <c r="A104" t="s">
         <v>212</v>
       </c>
@@ -3247,7 +3254,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3">
       <c r="A105" t="s">
         <v>214</v>
       </c>
@@ -3258,7 +3265,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3">
       <c r="A106" t="s">
         <v>216</v>
       </c>
@@ -3269,7 +3276,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3">
       <c r="A107" t="s">
         <v>246</v>
       </c>
@@ -3280,7 +3287,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:3">
       <c r="A108" t="s">
         <v>218</v>
       </c>
@@ -3291,7 +3298,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3">
       <c r="A109" t="s">
         <v>220</v>
       </c>
@@ -3302,7 +3309,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:3">
       <c r="A110" t="s">
         <v>222</v>
       </c>
@@ -3313,7 +3320,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:3">
       <c r="A111" t="s">
         <v>224</v>
       </c>
@@ -3324,7 +3331,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:3">
       <c r="A112" t="s">
         <v>226</v>
       </c>
@@ -3335,7 +3342,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:5">
       <c r="A113" t="s">
         <v>228</v>
       </c>
@@ -3346,7 +3353,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:5">
       <c r="A114" t="s">
         <v>230</v>
       </c>
@@ -3357,7 +3364,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:5">
       <c r="A115" t="s">
         <v>232</v>
       </c>
@@ -3368,7 +3375,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:5">
       <c r="A116" t="s">
         <v>234</v>
       </c>
@@ -3379,7 +3386,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:5">
       <c r="A117" t="s">
         <v>236</v>
       </c>
@@ -3390,7 +3397,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:5">
       <c r="A118" t="s">
         <v>238</v>
       </c>
@@ -3401,7 +3408,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:5">
       <c r="A119" t="s">
         <v>240</v>
       </c>
@@ -3412,7 +3419,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:5">
       <c r="A120" t="s">
         <v>242</v>
       </c>
@@ -3423,7 +3430,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:5">
       <c r="A121" t="s">
         <v>244</v>
       </c>
@@ -3434,7 +3441,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:5">
       <c r="A122" t="s">
         <v>248</v>
       </c>
@@ -3445,7 +3452,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:5">
       <c r="A123" t="s">
         <v>250</v>
       </c>
@@ -3456,7 +3463,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:5">
       <c r="A124" t="s">
         <v>252</v>
       </c>
@@ -3467,7 +3474,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:5">
       <c r="A125" t="s">
         <v>253</v>
       </c>
@@ -3478,7 +3485,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:5">
       <c r="A126" t="s">
         <v>256</v>
       </c>
@@ -3492,7 +3499,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:5">
       <c r="A127" t="s">
         <v>258</v>
       </c>
@@ -3503,7 +3510,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:5">
       <c r="A128" t="s">
         <v>260</v>
       </c>
@@ -3514,7 +3521,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:3">
       <c r="A129" s="1" t="s">
         <v>262</v>
       </c>
@@ -3525,7 +3532,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:3">
       <c r="A130" s="1" t="s">
         <v>265</v>
       </c>
@@ -3536,7 +3543,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:3">
       <c r="A131" s="1" t="s">
         <v>267</v>
       </c>
@@ -3547,7 +3554,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:3">
       <c r="A132" s="2" t="s">
         <v>268</v>
       </c>
@@ -3558,7 +3565,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:3">
       <c r="A133" s="2" t="s">
         <v>269</v>
       </c>
@@ -3569,7 +3576,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:3">
       <c r="A134" s="2" t="s">
         <v>270</v>
       </c>
@@ -3580,7 +3587,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:3" ht="16">
       <c r="A135" s="2" t="s">
         <v>271</v>
       </c>
@@ -3591,7 +3598,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:3" ht="16">
       <c r="A136" s="2" t="s">
         <v>272</v>
       </c>
@@ -3602,7 +3609,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:3" ht="16">
       <c r="A137" s="2" t="s">
         <v>273</v>
       </c>
@@ -3613,7 +3620,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:3" ht="16">
       <c r="A138" s="2" t="s">
         <v>274</v>
       </c>
@@ -3624,7 +3631,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:3">
       <c r="A139" s="3" t="s">
         <v>275</v>
       </c>
@@ -3635,7 +3642,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:3">
       <c r="A140" s="3" t="s">
         <v>276</v>
       </c>
@@ -3646,7 +3653,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:3">
       <c r="A141" s="3" t="s">
         <v>277</v>
       </c>
@@ -3657,7 +3664,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:3">
       <c r="A142" s="1" t="s">
         <v>288</v>
       </c>
@@ -3668,7 +3675,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:3">
       <c r="A143" t="s">
         <v>290</v>
       </c>
@@ -3679,7 +3686,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:3">
       <c r="A144" s="1" t="s">
         <v>292</v>
       </c>
@@ -3690,7 +3697,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:5">
       <c r="A145" s="1" t="s">
         <v>296</v>
       </c>
@@ -3701,7 +3708,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:5">
       <c r="A146" s="1" t="s">
         <v>297</v>
       </c>
@@ -3712,7 +3719,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:5">
       <c r="A147" s="1" t="s">
         <v>302</v>
       </c>
@@ -3723,7 +3730,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:5">
       <c r="A148" s="1" t="s">
         <v>303</v>
       </c>
@@ -3734,7 +3741,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:5">
       <c r="A149" s="1" t="s">
         <v>304</v>
       </c>
@@ -3745,7 +3752,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:5">
       <c r="A150" s="1" t="s">
         <v>305</v>
       </c>
@@ -3756,7 +3763,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:5">
       <c r="A151" t="s">
         <v>307</v>
       </c>
@@ -3767,7 +3774,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:5">
       <c r="A152" t="s">
         <v>308</v>
       </c>
@@ -3778,7 +3785,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:5">
       <c r="A153" t="s">
         <v>310</v>
       </c>
@@ -3792,7 +3799,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:5">
       <c r="A154" t="s">
         <v>311</v>
       </c>
@@ -3803,7 +3810,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:5">
       <c r="A155" t="s">
         <v>315</v>
       </c>
@@ -3814,7 +3821,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:5" ht="16">
       <c r="A156" t="s">
         <v>316</v>
       </c>
@@ -3825,7 +3832,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:5">
       <c r="A157" t="s">
         <v>319</v>
       </c>
@@ -3836,7 +3843,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:5">
       <c r="A158" t="s">
         <v>320</v>
       </c>
@@ -3847,7 +3854,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:5">
       <c r="A159" t="s">
         <v>323</v>
       </c>
@@ -3858,7 +3865,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:5">
       <c r="A160" t="s">
         <v>324</v>
       </c>
@@ -3869,7 +3876,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:3">
       <c r="A161" t="s">
         <v>326</v>
       </c>
@@ -3880,7 +3887,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:3">
       <c r="A162" s="1" t="s">
         <v>328</v>
       </c>
@@ -3891,7 +3898,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:3">
       <c r="A163" t="s">
         <v>330</v>
       </c>
@@ -3902,7 +3909,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:3">
       <c r="A164" t="s">
         <v>333</v>
       </c>
@@ -3913,7 +3920,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:3">
       <c r="A165" s="1" t="s">
         <v>344</v>
       </c>
@@ -3924,7 +3931,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:3">
       <c r="A166" s="1" t="s">
         <v>345</v>
       </c>
@@ -3935,7 +3942,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:3">
       <c r="A167" s="1" t="s">
         <v>346</v>
       </c>
@@ -3946,7 +3953,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:3">
       <c r="A168" s="1" t="s">
         <v>347</v>
       </c>
@@ -3957,7 +3964,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:3">
       <c r="A169" s="1" t="s">
         <v>348</v>
       </c>
@@ -3968,7 +3975,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:3">
       <c r="A170" s="1" t="s">
         <v>349</v>
       </c>
@@ -3979,7 +3986,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:3">
       <c r="A171" s="1" t="s">
         <v>350</v>
       </c>
@@ -3990,7 +3997,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:3">
       <c r="A172" s="1" t="s">
         <v>351</v>
       </c>
@@ -4001,7 +4008,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:3">
       <c r="A173" s="1" t="s">
         <v>352</v>
       </c>
@@ -4012,7 +4019,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:3">
       <c r="A174" s="1" t="s">
         <v>353</v>
       </c>
@@ -4023,7 +4030,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:3">
       <c r="A175" t="s">
         <v>354</v>
       </c>
@@ -4034,7 +4041,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:3">
       <c r="A176" s="9" t="s">
         <v>356</v>
       </c>
@@ -4045,7 +4052,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:3">
       <c r="A177" s="9" t="s">
         <v>358</v>
       </c>
@@ -4056,7 +4063,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:3">
       <c r="A178" s="9" t="s">
         <v>360</v>
       </c>
@@ -4067,7 +4074,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:3">
       <c r="A179" s="9" t="s">
         <v>362</v>
       </c>
@@ -4078,7 +4085,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:3">
       <c r="A180" s="9" t="s">
         <v>364</v>
       </c>
@@ -4089,7 +4096,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:3">
       <c r="A181" s="9" t="s">
         <v>366</v>
       </c>
@@ -4100,7 +4107,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:3">
       <c r="A182" s="9" t="s">
         <v>368</v>
       </c>
@@ -4111,7 +4118,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:3">
       <c r="A183" s="9" t="s">
         <v>370</v>
       </c>
@@ -4122,7 +4129,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:3">
       <c r="A184" s="9" t="s">
         <v>372</v>
       </c>
@@ -4133,7 +4140,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:3">
       <c r="A185" s="9" t="s">
         <v>374</v>
       </c>
@@ -4144,7 +4151,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:3">
       <c r="A186" s="9" t="s">
         <v>376</v>
       </c>
@@ -4155,7 +4162,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:3">
       <c r="A187" s="9" t="s">
         <v>378</v>
       </c>
@@ -4166,7 +4173,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:3">
       <c r="A188" s="9" t="s">
         <v>380</v>
       </c>
@@ -4177,7 +4184,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:3">
       <c r="A189" s="9" t="s">
         <v>382</v>
       </c>
@@ -4188,7 +4195,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:3">
       <c r="A190" s="9" t="s">
         <v>384</v>
       </c>
@@ -4199,7 +4206,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:3">
       <c r="A191" s="9" t="s">
         <v>386</v>
       </c>
@@ -4210,7 +4217,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:3">
       <c r="A192" s="9" t="s">
         <v>388</v>
       </c>
@@ -4221,7 +4228,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:3">
       <c r="A193" s="9" t="s">
         <v>390</v>
       </c>
@@ -4232,7 +4239,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:3">
       <c r="A194" s="9" t="s">
         <v>392</v>
       </c>
@@ -4243,7 +4250,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:3">
       <c r="A195" s="9" t="s">
         <v>394</v>
       </c>
@@ -4254,7 +4261,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:3">
       <c r="A196" s="9" t="s">
         <v>396</v>
       </c>
@@ -4265,7 +4272,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:3">
       <c r="A197" s="9" t="s">
         <v>398</v>
       </c>
@@ -4276,7 +4283,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:3">
       <c r="A198" s="9" t="s">
         <v>400</v>
       </c>
@@ -4287,7 +4294,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:3">
       <c r="A199" s="9" t="s">
         <v>402</v>
       </c>
@@ -4298,7 +4305,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:3">
       <c r="A200" s="9" t="s">
         <v>404</v>
       </c>
@@ -4309,7 +4316,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:3">
       <c r="A201" s="9" t="s">
         <v>406</v>
       </c>
@@ -4320,7 +4327,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:3">
       <c r="A202" s="9" t="s">
         <v>408</v>
       </c>
@@ -4331,7 +4338,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:3">
       <c r="A203" s="9" t="s">
         <v>410</v>
       </c>
@@ -4342,7 +4349,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:3">
       <c r="A204" s="9" t="s">
         <v>412</v>
       </c>
@@ -4353,7 +4360,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:3">
       <c r="A205" s="9" t="s">
         <v>414</v>
       </c>
@@ -4364,7 +4371,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:3">
       <c r="A206" s="9" t="s">
         <v>416</v>
       </c>
@@ -4375,7 +4382,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:3">
       <c r="A207" s="9" t="s">
         <v>418</v>
       </c>
@@ -4386,7 +4393,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:3">
       <c r="A208" s="9" t="s">
         <v>420</v>
       </c>
@@ -4397,7 +4404,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:3">
       <c r="A209" s="9" t="s">
         <v>422</v>
       </c>
@@ -4408,7 +4415,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:3">
       <c r="A210" s="9" t="s">
         <v>424</v>
       </c>
@@ -4419,7 +4426,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:3">
       <c r="A211" s="9" t="s">
         <v>426</v>
       </c>
@@ -4430,7 +4437,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:3">
       <c r="A212" s="9" t="s">
         <v>428</v>
       </c>
@@ -4441,7 +4448,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:3">
       <c r="A213" s="9" t="s">
         <v>430</v>
       </c>
@@ -4452,7 +4459,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:3">
       <c r="A214" s="9" t="s">
         <v>432</v>
       </c>
@@ -4463,7 +4470,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:3">
       <c r="A215" s="9" t="s">
         <v>434</v>
       </c>
@@ -4474,7 +4481,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:3">
       <c r="A216" s="9" t="s">
         <v>436</v>
       </c>
@@ -4485,7 +4492,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:3">
       <c r="A217" s="9" t="s">
         <v>438</v>
       </c>
@@ -4496,7 +4503,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:3">
       <c r="A218" s="9" t="s">
         <v>440</v>
       </c>
@@ -4507,7 +4514,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:3">
       <c r="A219" s="9" t="s">
         <v>442</v>
       </c>
@@ -4518,7 +4525,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:3">
       <c r="A220" s="9" t="s">
         <v>444</v>
       </c>
@@ -4529,7 +4536,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:3">
       <c r="A221" s="9" t="s">
         <v>446</v>
       </c>
@@ -4540,7 +4547,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:3">
       <c r="A222" s="9" t="s">
         <v>448</v>
       </c>
@@ -4551,7 +4558,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:3">
       <c r="A223" s="9" t="s">
         <v>450</v>
       </c>
@@ -4562,7 +4569,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:3">
       <c r="A224" s="9" t="s">
         <v>452</v>
       </c>
@@ -4573,7 +4580,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:3">
       <c r="A225" s="9" t="s">
         <v>454</v>
       </c>
@@ -4584,7 +4591,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:3">
       <c r="A226" s="9" t="s">
         <v>456</v>
       </c>
@@ -4595,7 +4602,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:3">
       <c r="A227" s="9" t="s">
         <v>458</v>
       </c>
@@ -4606,7 +4613,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:3">
       <c r="A228" s="9" t="s">
         <v>460</v>
       </c>
@@ -4617,7 +4624,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:3">
       <c r="A229" s="9" t="s">
         <v>462</v>
       </c>
@@ -4628,7 +4635,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:3">
       <c r="A230" s="9" t="s">
         <v>464</v>
       </c>
@@ -4639,7 +4646,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:3">
       <c r="A231" s="9" t="s">
         <v>466</v>
       </c>
@@ -4650,7 +4657,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:3">
       <c r="A232" s="9" t="s">
         <v>468</v>
       </c>
@@ -4661,7 +4668,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:3">
       <c r="A233" s="9" t="s">
         <v>470</v>
       </c>
@@ -4672,7 +4679,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:3">
       <c r="A234" s="9" t="s">
         <v>472</v>
       </c>
@@ -4683,7 +4690,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:3">
       <c r="A235" s="9" t="s">
         <v>474</v>
       </c>
@@ -4694,7 +4701,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:3">
       <c r="A236" s="9" t="s">
         <v>476</v>
       </c>
@@ -4705,7 +4712,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:3">
       <c r="A237" s="9" t="s">
         <v>478</v>
       </c>
@@ -4716,7 +4723,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:3">
       <c r="A238" s="9" t="s">
         <v>480</v>
       </c>
@@ -4727,7 +4734,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:3">
       <c r="A239" s="9" t="s">
         <v>482</v>
       </c>
@@ -4738,7 +4745,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:3">
       <c r="A240" s="9" t="s">
         <v>484</v>
       </c>
@@ -4749,7 +4756,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:3">
       <c r="A241" s="9" t="s">
         <v>486</v>
       </c>
@@ -4760,7 +4767,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:3">
       <c r="A242" s="9" t="s">
         <v>488</v>
       </c>
@@ -4771,7 +4778,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:3">
       <c r="A243" s="9" t="s">
         <v>490</v>
       </c>
@@ -4782,7 +4789,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:3">
       <c r="A244" s="9" t="s">
         <v>492</v>
       </c>
@@ -4793,7 +4800,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:3">
       <c r="A245" s="9" t="s">
         <v>494</v>
       </c>
@@ -4804,7 +4811,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:3">
       <c r="A246" s="9" t="s">
         <v>496</v>
       </c>
@@ -4815,7 +4822,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:3">
       <c r="A247" s="9" t="s">
         <v>498</v>
       </c>
@@ -4826,7 +4833,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:3">
       <c r="A248" s="9" t="s">
         <v>500</v>
       </c>
@@ -4837,7 +4844,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:3">
       <c r="A249" s="9" t="s">
         <v>502</v>
       </c>
@@ -4848,7 +4855,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:3">
       <c r="A250" s="9" t="s">
         <v>504</v>
       </c>
@@ -4859,7 +4866,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:3">
       <c r="A251" s="9" t="s">
         <v>506</v>
       </c>
@@ -4870,7 +4877,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:3">
       <c r="A252" s="9" t="s">
         <v>508</v>
       </c>
@@ -4881,7 +4888,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:3">
       <c r="A253" s="9" t="s">
         <v>510</v>
       </c>
@@ -4892,7 +4899,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:3">
       <c r="A254" s="9" t="s">
         <v>512</v>
       </c>
@@ -4903,7 +4910,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:3">
       <c r="A255" s="9" t="s">
         <v>514</v>
       </c>
@@ -4914,7 +4921,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:3">
       <c r="A256" s="9" t="s">
         <v>516</v>
       </c>
@@ -4925,7 +4932,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:3">
       <c r="A257" s="9" t="s">
         <v>518</v>
       </c>
@@ -4936,7 +4943,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:3">
       <c r="A258" s="9" t="s">
         <v>520</v>
       </c>
@@ -4947,7 +4954,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:3">
       <c r="A259" s="9" t="s">
         <v>522</v>
       </c>
@@ -4958,7 +4965,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:3">
       <c r="A260" s="9" t="s">
         <v>524</v>
       </c>
@@ -4969,7 +4976,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:3">
       <c r="A261" s="9" t="s">
         <v>526</v>
       </c>
@@ -4980,7 +4987,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:3">
       <c r="A262" s="9" t="s">
         <v>528</v>
       </c>
@@ -4991,7 +4998,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:3">
       <c r="A263" s="9" t="s">
         <v>530</v>
       </c>
@@ -5002,7 +5009,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:3">
       <c r="A264" s="9" t="s">
         <v>532</v>
       </c>
@@ -5013,7 +5020,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:3">
       <c r="A265" s="9" t="s">
         <v>534</v>
       </c>
@@ -5024,7 +5031,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:3">
       <c r="A266" s="9" t="s">
         <v>536</v>
       </c>
@@ -5035,7 +5042,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:3">
       <c r="A267" s="9" t="s">
         <v>538</v>
       </c>
@@ -5046,7 +5053,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:3">
       <c r="A268" t="s">
         <v>540</v>
       </c>
@@ -5055,6 +5062,17 @@
       </c>
       <c r="C268" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3">
+      <c r="A269" t="s">
+        <v>542</v>
+      </c>
+      <c r="B269" t="s">
+        <v>543</v>
+      </c>
+      <c r="C269" t="s">
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -5062,39 +5080,39 @@
     <sortCondition ref="B2:B50"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="A129" r:id="rId1"/>
-    <hyperlink ref="A130" r:id="rId2"/>
-    <hyperlink ref="A131" r:id="rId3"/>
-    <hyperlink ref="B131" r:id="rId4" display="http://purl.obolibrary.org/obo/OBI_0001930 categorical value specification"/>
-    <hyperlink ref="A132" r:id="rId5"/>
-    <hyperlink ref="A133" r:id="rId6"/>
-    <hyperlink ref="A134" r:id="rId7"/>
-    <hyperlink ref="A135" r:id="rId8"/>
-    <hyperlink ref="A136" r:id="rId9"/>
-    <hyperlink ref="A137" r:id="rId10"/>
-    <hyperlink ref="A138" r:id="rId11"/>
-    <hyperlink ref="A139" r:id="rId12"/>
-    <hyperlink ref="A140" r:id="rId13"/>
-    <hyperlink ref="A141" r:id="rId14"/>
-    <hyperlink ref="A142" r:id="rId15"/>
-    <hyperlink ref="A144" r:id="rId16"/>
-    <hyperlink ref="A145" r:id="rId17"/>
-    <hyperlink ref="A146" r:id="rId18"/>
-    <hyperlink ref="A147" r:id="rId19"/>
-    <hyperlink ref="A148" r:id="rId20"/>
-    <hyperlink ref="A149" r:id="rId21"/>
-    <hyperlink ref="A150" r:id="rId22"/>
-    <hyperlink ref="A162" r:id="rId23"/>
-    <hyperlink ref="A165" r:id="rId24"/>
-    <hyperlink ref="A166" r:id="rId25"/>
-    <hyperlink ref="A167" r:id="rId26"/>
-    <hyperlink ref="A168" r:id="rId27"/>
-    <hyperlink ref="A169" r:id="rId28"/>
-    <hyperlink ref="A170" r:id="rId29"/>
-    <hyperlink ref="A171" r:id="rId30"/>
-    <hyperlink ref="A172" r:id="rId31"/>
-    <hyperlink ref="A173" r:id="rId32"/>
-    <hyperlink ref="A174" r:id="rId33"/>
+    <hyperlink ref="A129" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A130" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A131" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B131" r:id="rId4" display="http://purl.obolibrary.org/obo/OBI_0001930 categorical value specification" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="A132" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="A133" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="A134" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="A135" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="A136" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="A137" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="A138" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="A139" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="A140" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="A141" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="A142" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="A144" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="A145" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="A146" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="A147" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="A148" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="A149" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="A150" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="A162" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="A165" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="A166" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="A167" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="A168" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="A169" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="A170" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="A171" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="A172" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="A173" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="A174" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -5102,24 +5120,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated ontodog files to get OBI terms described in #7, #14, #55
</commit_message>
<xml_diff>
--- a/src/external/ontoDog_input/ontoDog_input.xlsx
+++ b/src/external/ontoDog_input/ontoDog_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10609"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stoeckrt/Git/biobanking/ontology/src/external/ontoDog_input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E8E695-2701-3B46-A6F6-FCDD59A58970}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D4A8E3-3667-3A40-B0A5-75F614898DB0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35460" yWindow="3860" windowWidth="32880" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="548">
   <si>
     <t>Homo sapiens</t>
   </si>
@@ -1662,6 +1662,18 @@
   </si>
   <si>
     <t>time unit</t>
+  </si>
+  <si>
+    <t>FFPE specimen</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_1200000</t>
+  </si>
+  <si>
+    <t>swab specimen</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0002599</t>
   </si>
 </sst>
 </file>
@@ -2077,10 +2089,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E269"/>
+  <dimension ref="A1:E271"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A261" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D273" sqref="D273"/>
+    <sheetView tabSelected="1" topLeftCell="A249" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A272" sqref="A272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -4932,7 +4944,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="257" spans="1:3">
+    <row r="257" spans="1:5">
       <c r="A257" s="9" t="s">
         <v>518</v>
       </c>
@@ -4943,7 +4955,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="258" spans="1:3">
+    <row r="258" spans="1:5">
       <c r="A258" s="9" t="s">
         <v>520</v>
       </c>
@@ -4954,7 +4966,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="259" spans="1:3">
+    <row r="259" spans="1:5">
       <c r="A259" s="9" t="s">
         <v>522</v>
       </c>
@@ -4965,7 +4977,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="260" spans="1:3">
+    <row r="260" spans="1:5">
       <c r="A260" s="9" t="s">
         <v>524</v>
       </c>
@@ -4976,7 +4988,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="261" spans="1:3">
+    <row r="261" spans="1:5">
       <c r="A261" s="9" t="s">
         <v>526</v>
       </c>
@@ -4987,7 +4999,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="262" spans="1:3">
+    <row r="262" spans="1:5">
       <c r="A262" s="9" t="s">
         <v>528</v>
       </c>
@@ -4998,7 +5010,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="263" spans="1:3">
+    <row r="263" spans="1:5">
       <c r="A263" s="9" t="s">
         <v>530</v>
       </c>
@@ -5009,7 +5021,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="264" spans="1:3">
+    <row r="264" spans="1:5">
       <c r="A264" s="9" t="s">
         <v>532</v>
       </c>
@@ -5020,7 +5032,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="265" spans="1:3">
+    <row r="265" spans="1:5">
       <c r="A265" s="9" t="s">
         <v>534</v>
       </c>
@@ -5031,7 +5043,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="266" spans="1:3">
+    <row r="266" spans="1:5">
       <c r="A266" s="9" t="s">
         <v>536</v>
       </c>
@@ -5042,7 +5054,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="267" spans="1:3">
+    <row r="267" spans="1:5">
       <c r="A267" s="9" t="s">
         <v>538</v>
       </c>
@@ -5053,7 +5065,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="268" spans="1:3">
+    <row r="268" spans="1:5">
       <c r="A268" t="s">
         <v>540</v>
       </c>
@@ -5064,7 +5076,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="269" spans="1:3">
+    <row r="269" spans="1:5">
       <c r="A269" t="s">
         <v>542</v>
       </c>
@@ -5073,6 +5085,31 @@
       </c>
       <c r="C269" t="s">
         <v>209</v>
+      </c>
+    </row>
+    <row r="270" spans="1:5">
+      <c r="A270" t="s">
+        <v>545</v>
+      </c>
+      <c r="B270" t="s">
+        <v>544</v>
+      </c>
+      <c r="C270" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="271" spans="1:5">
+      <c r="A271" t="s">
+        <v>547</v>
+      </c>
+      <c r="B271" t="s">
+        <v>546</v>
+      </c>
+      <c r="C271" t="s">
+        <v>85</v>
+      </c>
+      <c r="E271" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Import MIABIS requested terms from OBI
</commit_message>
<xml_diff>
--- a/src/external/ontoDog_input/ontoDog_input.xlsx
+++ b/src/external/ontoDog_input/ontoDog_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11013"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stoeckrt/Git/biobanking/ontology/src/external/ontoDog_input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarah.bost/Desktop/Git_Repositories/ontology/src/external/ontoDog_input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D4A8E3-3667-3A40-B0A5-75F614898DB0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C647F0BD-4BF6-0048-AB04-CA7A313727FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20680" yWindow="3400" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="558">
   <si>
     <t>Homo sapiens</t>
   </si>
@@ -1674,6 +1674,36 @@
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/OBI_0002599</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0002614</t>
+  </si>
+  <si>
+    <t>birth cohort study design</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0002615</t>
+  </si>
+  <si>
+    <t>disease specific study design</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0002618</t>
+  </si>
+  <si>
+    <t>national biomedical registry</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0002617</t>
+  </si>
+  <si>
+    <t>national registry</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0002616</t>
+  </si>
+  <si>
+    <t>genealogical record</t>
   </si>
 </sst>
 </file>
@@ -1762,7 +1792,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1779,6 +1809,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
@@ -2089,10 +2120,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E271"/>
+  <dimension ref="A1:E276"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A249" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A272" sqref="A272"/>
+    <sheetView tabSelected="1" topLeftCell="A253" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A272" sqref="A272:A276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -5110,6 +5141,61 @@
       </c>
       <c r="E271" t="s">
         <v>84</v>
+      </c>
+    </row>
+    <row r="272" spans="1:5" ht="16">
+      <c r="A272" s="10" t="s">
+        <v>548</v>
+      </c>
+      <c r="B272" s="8" t="s">
+        <v>549</v>
+      </c>
+      <c r="C272" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3">
+      <c r="A273" s="10" t="s">
+        <v>550</v>
+      </c>
+      <c r="B273" t="s">
+        <v>551</v>
+      </c>
+      <c r="C273" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3">
+      <c r="A274" s="10" t="s">
+        <v>552</v>
+      </c>
+      <c r="B274" t="s">
+        <v>553</v>
+      </c>
+      <c r="C274" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3">
+      <c r="A275" s="10" t="s">
+        <v>554</v>
+      </c>
+      <c r="B275" t="s">
+        <v>555</v>
+      </c>
+      <c r="C275" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3">
+      <c r="A276" s="10" t="s">
+        <v>556</v>
+      </c>
+      <c r="B276" t="s">
+        <v>557</v>
+      </c>
+      <c r="C276" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
delete birth cohort study design from OntoDog
</commit_message>
<xml_diff>
--- a/src/external/ontoDog_input/ontoDog_input.xlsx
+++ b/src/external/ontoDog_input/ontoDog_input.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10308"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarah.bost/Desktop/Git_Repositories/ontology/src/external/ontoDog_input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarah.bost/Desktop/Git_Repositories/obib/ontology/src/external/ontoDog_input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C647F0BD-4BF6-0048-AB04-CA7A313727FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B496AC-3C33-2D40-AA89-36BA93FDEE6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20680" yWindow="3400" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="558">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="556">
   <si>
     <t>Homo sapiens</t>
   </si>
@@ -1674,12 +1674,6 @@
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/OBI_0002599</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/OBI_0002614</t>
-  </si>
-  <si>
-    <t>birth cohort study design</t>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/OBI_0002615</t>
@@ -1739,26 +1733,31 @@
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2120,10 +2119,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E276"/>
+  <dimension ref="A1:E275"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A253" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A272" sqref="A272:A276"/>
+      <selection activeCell="D264" sqref="D264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -5143,11 +5142,11 @@
         <v>84</v>
       </c>
     </row>
-    <row r="272" spans="1:5" ht="16">
+    <row r="272" spans="1:5">
       <c r="A272" s="10" t="s">
         <v>548</v>
       </c>
-      <c r="B272" s="8" t="s">
+      <c r="B272" t="s">
         <v>549</v>
       </c>
       <c r="C272" t="s">
@@ -5187,19 +5186,8 @@
         <v>85</v>
       </c>
     </row>
-    <row r="276" spans="1:3">
-      <c r="A276" s="10" t="s">
-        <v>556</v>
-      </c>
-      <c r="B276" t="s">
-        <v>557</v>
-      </c>
-      <c r="C276" t="s">
-        <v>85</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState ref="A2:E50">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E50">
     <sortCondition ref="B2:B50"/>
   </sortState>
   <hyperlinks>

</xml_diff>

<commit_message>
delete 'birth cohort study design' from ontoDog_input.xlsx
</commit_message>
<xml_diff>
--- a/src/external/ontoDog_input/ontoDog_input.xlsx
+++ b/src/external/ontoDog_input/ontoDog_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10308"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarah.bost/Desktop/Git_Repositories/ontology/src/external/ontoDog_input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarah.bost/Desktop/Git_Repositories/obib/ontology/src/external/ontoDog_input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C647F0BD-4BF6-0048-AB04-CA7A313727FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F18FD2-254D-7543-8B17-9CCB3D8926DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20680" yWindow="3400" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="558">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="556">
   <si>
     <t>Homo sapiens</t>
   </si>
@@ -1674,12 +1674,6 @@
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/OBI_0002599</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/OBI_0002614</t>
-  </si>
-  <si>
-    <t>birth cohort study design</t>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/OBI_0002615</t>
@@ -1739,26 +1733,31 @@
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2120,10 +2119,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E276"/>
+  <dimension ref="A1:E275"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A253" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A272" sqref="A272:A276"/>
+      <selection activeCell="E263" sqref="E263"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -5143,11 +5142,11 @@
         <v>84</v>
       </c>
     </row>
-    <row r="272" spans="1:5" ht="16">
+    <row r="272" spans="1:5">
       <c r="A272" s="10" t="s">
         <v>548</v>
       </c>
-      <c r="B272" s="8" t="s">
+      <c r="B272" t="s">
         <v>549</v>
       </c>
       <c r="C272" t="s">
@@ -5187,19 +5186,8 @@
         <v>85</v>
       </c>
     </row>
-    <row r="276" spans="1:3">
-      <c r="A276" s="10" t="s">
-        <v>556</v>
-      </c>
-      <c r="B276" t="s">
-        <v>557</v>
-      </c>
-      <c r="C276" t="s">
-        <v>85</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState ref="A2:E50">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E50">
     <sortCondition ref="B2:B50"/>
   </sortState>
   <hyperlinks>

</xml_diff>

<commit_message>
change 'postal code of biobank contact' axioms to remove 'obsolete_postal code'
</commit_message>
<xml_diff>
--- a/src/external/ontoDog_input/ontoDog_input.xlsx
+++ b/src/external/ontoDog_input/ontoDog_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarah.bost/Desktop/Git_Repositories/obib/ontology/src/external/ontoDog_input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F18FD2-254D-7543-8B17-9CCB3D8926DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF0F7F6-2DE9-6842-B3D9-3FCB3A680E48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31100" yWindow="800" windowWidth="33600" windowHeight="19120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="558">
   <si>
     <t>Homo sapiens</t>
   </si>
@@ -1698,6 +1698,12 @@
   </si>
   <si>
     <t>genealogical record</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/IAO_0000646</t>
+  </si>
+  <si>
+    <t>postal code</t>
   </si>
 </sst>
 </file>
@@ -2119,10 +2125,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E275"/>
+  <dimension ref="A1:E276"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A253" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E263" sqref="E263"/>
+    <sheetView tabSelected="1" topLeftCell="A261" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B276" sqref="B276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -5183,6 +5189,17 @@
         <v>555</v>
       </c>
       <c r="C275" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3">
+      <c r="A276" s="10" t="s">
+        <v>556</v>
+      </c>
+      <c r="B276" t="s">
+        <v>557</v>
+      </c>
+      <c r="C276" t="s">
         <v>85</v>
       </c>
     </row>

</xml_diff>

<commit_message>
replaced ERO biopsy with OBI biopsy, obsoleted OBIB needle biopsies, imported other related and specimen terms as per issue #76
</commit_message>
<xml_diff>
--- a/src/external/ontoDog_input/ontoDog_input.xlsx
+++ b/src/external/ontoDog_input/ontoDog_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarah.bost/Desktop/Git_Repositories/obib/ontology/src/external/ontoDog_input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stoeckrt/Git/biobanking/ontology/src/external/ontoDog_input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF0F7F6-2DE9-6842-B3D9-3FCB3A680E48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2DBF989-5306-784D-8549-6439AEEF623F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31100" yWindow="800" windowWidth="33600" windowHeight="19120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19080" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="558">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="602">
   <si>
     <t>Homo sapiens</t>
   </si>
@@ -1704,6 +1704,138 @@
   </si>
   <si>
     <t>postal code</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0002650</t>
+  </si>
+  <si>
+    <t>biopsy</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0002775</t>
+  </si>
+  <si>
+    <t>platelet-poor plasma preparation process</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0000436</t>
+  </si>
+  <si>
+    <t>needle</t>
+  </si>
+  <si>
+    <t>uterine cervix specimen</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_2000000</t>
+  </si>
+  <si>
+    <t>urethra specimen</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_2000001</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_2000018</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_2000017</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_2000002</t>
+  </si>
+  <si>
+    <t>cervical mucus specimen</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_2000003</t>
+  </si>
+  <si>
+    <t>throat specimen</t>
+  </si>
+  <si>
+    <t>eye</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_2000004</t>
+  </si>
+  <si>
+    <t>respiratory system specimen</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_2000005</t>
+  </si>
+  <si>
+    <t>upper respiratory tract specimen</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_2000006</t>
+  </si>
+  <si>
+    <t>nasopharynx specimen</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_2000007</t>
+  </si>
+  <si>
+    <t>semen specimen</t>
+  </si>
+  <si>
+    <t>bodily fluid specimen</t>
+  </si>
+  <si>
+    <t>chrorionic villus specimen</t>
+  </si>
+  <si>
+    <t>meconium specimen</t>
+  </si>
+  <si>
+    <t>umbilical cord blood specimen</t>
+  </si>
+  <si>
+    <t>arterial blood specimen</t>
+  </si>
+  <si>
+    <t>venous blood specimen</t>
+  </si>
+  <si>
+    <t>capillary blood specimen</t>
+  </si>
+  <si>
+    <t>erythrocyte specimen</t>
+  </si>
+  <si>
+    <t>reticulocyte specimen</t>
+  </si>
+  <si>
+    <t>leukocyte specimen</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_2000008</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_2000009</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_2000010</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_2000011</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_2000012</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_2000013</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_2000014</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_2000015</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_2000016</t>
   </si>
 </sst>
 </file>
@@ -1797,7 +1929,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1815,6 +1947,7 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
@@ -2125,15 +2258,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E276"/>
+  <dimension ref="A1:E298"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A261" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B276" sqref="B276"/>
+    <sheetView tabSelected="1" topLeftCell="A276" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C298" sqref="C298"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="57" customWidth="1"/>
+    <col min="1" max="1" width="38.5" customWidth="1"/>
     <col min="2" max="2" width="49.1640625" customWidth="1"/>
     <col min="3" max="3" width="18.33203125" customWidth="1"/>
     <col min="4" max="4" width="22.6640625" customWidth="1"/>
@@ -2200,6 +2333,9 @@
       <c r="C5" t="s">
         <v>85</v>
       </c>
+      <c r="E5" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
@@ -2862,7 +2998,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:5">
       <c r="A65" t="s">
         <v>172</v>
       </c>
@@ -2873,7 +3009,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:5">
       <c r="A66" t="s">
         <v>173</v>
       </c>
@@ -2884,7 +3020,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:5">
       <c r="A67" t="s">
         <v>174</v>
       </c>
@@ -2894,8 +3030,11 @@
       <c r="C67" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="68" spans="1:3">
+      <c r="E67" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
       <c r="A68" t="s">
         <v>175</v>
       </c>
@@ -2906,7 +3045,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:5">
       <c r="A69" t="s">
         <v>176</v>
       </c>
@@ -2917,7 +3056,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:5">
       <c r="A70" t="s">
         <v>177</v>
       </c>
@@ -2928,7 +3067,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:5">
       <c r="A71" t="s">
         <v>178</v>
       </c>
@@ -2939,7 +3078,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:5">
       <c r="A72" t="s">
         <v>179</v>
       </c>
@@ -2950,7 +3089,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:5">
       <c r="A73" t="s">
         <v>180</v>
       </c>
@@ -2961,7 +3100,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:5">
       <c r="A74" t="s">
         <v>181</v>
       </c>
@@ -2972,7 +3111,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:5">
       <c r="A75" t="s">
         <v>182</v>
       </c>
@@ -2983,7 +3122,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:5">
       <c r="A76" t="s">
         <v>183</v>
       </c>
@@ -2994,7 +3133,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:5">
       <c r="A77" t="s">
         <v>184</v>
       </c>
@@ -3005,7 +3144,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:5">
       <c r="A78" t="s">
         <v>185</v>
       </c>
@@ -3016,7 +3155,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:5">
       <c r="A79" t="s">
         <v>186</v>
       </c>
@@ -3027,7 +3166,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:5">
       <c r="A80" t="s">
         <v>187</v>
       </c>
@@ -5159,7 +5298,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="273" spans="1:3">
+    <row r="273" spans="1:5">
       <c r="A273" s="10" t="s">
         <v>550</v>
       </c>
@@ -5170,7 +5309,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="274" spans="1:3">
+    <row r="274" spans="1:5">
       <c r="A274" s="10" t="s">
         <v>552</v>
       </c>
@@ -5181,7 +5320,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="275" spans="1:3">
+    <row r="275" spans="1:5">
       <c r="A275" s="10" t="s">
         <v>554</v>
       </c>
@@ -5192,7 +5331,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="276" spans="1:3">
+    <row r="276" spans="1:5">
       <c r="A276" s="10" t="s">
         <v>556</v>
       </c>
@@ -5203,8 +5342,256 @@
         <v>85</v>
       </c>
     </row>
+    <row r="277" spans="1:5">
+      <c r="A277" s="11" t="s">
+        <v>558</v>
+      </c>
+      <c r="B277" t="s">
+        <v>559</v>
+      </c>
+      <c r="C277" t="s">
+        <v>85</v>
+      </c>
+      <c r="E277" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="278" spans="1:5">
+      <c r="A278" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="B278" t="s">
+        <v>563</v>
+      </c>
+      <c r="C278" t="s">
+        <v>85</v>
+      </c>
+      <c r="E278" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="279" spans="1:5">
+      <c r="A279" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="B279" t="s">
+        <v>561</v>
+      </c>
+      <c r="C279" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="280" spans="1:5">
+      <c r="A280" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="B280" t="s">
+        <v>564</v>
+      </c>
+      <c r="C280" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="281" spans="1:5">
+      <c r="A281" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="B281" t="s">
+        <v>566</v>
+      </c>
+      <c r="C281" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="282" spans="1:5">
+      <c r="A282" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="B282" t="s">
+        <v>571</v>
+      </c>
+      <c r="C282" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="283" spans="1:5">
+      <c r="A283" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="B283" t="s">
+        <v>573</v>
+      </c>
+      <c r="C283" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="284" spans="1:5">
+      <c r="A284" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="B284" t="s">
+        <v>574</v>
+      </c>
+      <c r="C284" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="285" spans="1:5">
+      <c r="A285" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="B285" t="s">
+        <v>576</v>
+      </c>
+      <c r="C285" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="286" spans="1:5">
+      <c r="A286" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="B286" t="s">
+        <v>578</v>
+      </c>
+      <c r="C286" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="287" spans="1:5">
+      <c r="A287" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="B287" t="s">
+        <v>580</v>
+      </c>
+      <c r="C287" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="288" spans="1:5">
+      <c r="A288" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="B288" t="s">
+        <v>582</v>
+      </c>
+      <c r="C288" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3">
+      <c r="A289" s="1" t="s">
+        <v>594</v>
+      </c>
+      <c r="B289" t="s">
+        <v>583</v>
+      </c>
+      <c r="C289" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3">
+      <c r="A290" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="B290" t="s">
+        <v>584</v>
+      </c>
+      <c r="C290" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3">
+      <c r="A291" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="B291" t="s">
+        <v>585</v>
+      </c>
+      <c r="C291" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3">
+      <c r="A292" s="1" t="s">
+        <v>597</v>
+      </c>
+      <c r="B292" t="s">
+        <v>586</v>
+      </c>
+      <c r="C292" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3">
+      <c r="A293" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="B293" t="s">
+        <v>587</v>
+      </c>
+      <c r="C293" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3">
+      <c r="A294" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="B294" t="s">
+        <v>588</v>
+      </c>
+      <c r="C294" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3">
+      <c r="A295" s="1" t="s">
+        <v>600</v>
+      </c>
+      <c r="B295" t="s">
+        <v>589</v>
+      </c>
+      <c r="C295" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3">
+      <c r="A296" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B296" t="s">
+        <v>590</v>
+      </c>
+      <c r="C296" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3">
+      <c r="A297" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="B297" t="s">
+        <v>591</v>
+      </c>
+      <c r="C297" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3">
+      <c r="A298" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="B298" t="s">
+        <v>592</v>
+      </c>
+      <c r="C298" t="s">
+        <v>85</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E50">
+  <sortState ref="A2:E50">
     <sortCondition ref="B2:B50"/>
   </sortState>
   <hyperlinks>
@@ -5241,6 +5628,28 @@
     <hyperlink ref="A172" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
     <hyperlink ref="A173" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
     <hyperlink ref="A174" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="A277" r:id="rId34" xr:uid="{757D2EB5-86BD-E541-B951-AA35BC37E6F2}"/>
+    <hyperlink ref="A278" r:id="rId35" xr:uid="{BA682A17-B422-7249-92AE-79C147A38FD0}"/>
+    <hyperlink ref="A279" r:id="rId36" xr:uid="{A2949D50-E667-614A-9534-D0D5F4CAC210}"/>
+    <hyperlink ref="A280" r:id="rId37" xr:uid="{B03E4E81-0AE5-4A48-86F2-7D059006664D}"/>
+    <hyperlink ref="A281" r:id="rId38" xr:uid="{3646357A-57A0-0C4E-A52A-F56E97131469}"/>
+    <hyperlink ref="A282" r:id="rId39" xr:uid="{D7621CA4-2BFE-C34E-B8E0-FC47E09E7B0A}"/>
+    <hyperlink ref="A283" r:id="rId40" xr:uid="{8615EA8C-ABE1-9E40-BF94-2C187658447C}"/>
+    <hyperlink ref="A284" r:id="rId41" xr:uid="{3DD60AE7-FFC9-6A49-9DFB-131CBA923AF6}"/>
+    <hyperlink ref="A285" r:id="rId42" xr:uid="{86DC5FB9-F293-684C-8843-BBFFE61A454F}"/>
+    <hyperlink ref="A286" r:id="rId43" xr:uid="{749DDD6E-77EA-F345-ACD0-5459A14B5410}"/>
+    <hyperlink ref="A287" r:id="rId44" xr:uid="{780373D2-6D34-C847-90B3-2F77E3F84847}"/>
+    <hyperlink ref="A288" r:id="rId45" xr:uid="{3B6D1476-9B63-534D-B11B-78B2358BB3EE}"/>
+    <hyperlink ref="A289" r:id="rId46" xr:uid="{EEB120FD-36D7-9E45-8E9C-B379485F743D}"/>
+    <hyperlink ref="A290" r:id="rId47" xr:uid="{1FAD7488-768C-BE4E-B67C-63F8383BF293}"/>
+    <hyperlink ref="A291" r:id="rId48" xr:uid="{E3118ADA-7700-8E42-AF8F-599F1F959F2C}"/>
+    <hyperlink ref="A292" r:id="rId49" xr:uid="{5E2821DB-B99E-AE44-B9D8-EB1C04DD34A7}"/>
+    <hyperlink ref="A293" r:id="rId50" xr:uid="{43C4E626-9153-4746-AF8F-332E248420EB}"/>
+    <hyperlink ref="A294" r:id="rId51" xr:uid="{494D8381-2C84-A848-B2CD-A2706C323457}"/>
+    <hyperlink ref="A295" r:id="rId52" xr:uid="{61602AD6-7390-4645-A3E8-1840E896FE30}"/>
+    <hyperlink ref="A296" r:id="rId53" xr:uid="{053AF680-CCE2-4745-B157-53C808FEEE59}"/>
+    <hyperlink ref="A297" r:id="rId54" xr:uid="{92E24047-3A57-9F49-A6AA-9549677D81C7}"/>
+    <hyperlink ref="A298" r:id="rId55" xr:uid="{0460BE5F-9CDC-8845-8C0E-75E98E940FFE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>